<commit_message>
Control module fixes + tests
</commit_message>
<xml_diff>
--- a/KPC8/Docs/Specs.xlsx
+++ b/KPC8/Docs/Specs.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Random\KPC8\KPC8\KPC8\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8DF2AC-2EF9-4277-9BCB-12B0747B3DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E11335C-D6B6-44E5-A7A5-432C953ACB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{17029D09-6E3C-4208-87C0-FA3EA582112B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="2" xr2:uid="{17029D09-6E3C-4208-87C0-FA3EA582112B}"/>
   </bookViews>
   <sheets>
-    <sheet name="16BitInstructionSet" sheetId="1" r:id="rId1"/>
-    <sheet name="Registers" sheetId="2" r:id="rId2"/>
-    <sheet name="Addressing" sheetId="3" r:id="rId3"/>
-    <sheet name="Control signals" sheetId="4" r:id="rId4"/>
+    <sheet name="Control signals" sheetId="4" r:id="rId1"/>
+    <sheet name="16BitInstructionSet" sheetId="1" r:id="rId2"/>
+    <sheet name="Registers" sheetId="2" r:id="rId3"/>
+    <sheet name="Addressing" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="121">
   <si>
     <t>OPCODE HEX</t>
   </si>
@@ -288,9 +288,6 @@
     <t>store byte in ram immediate</t>
   </si>
   <si>
-    <t>$z</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -324,18 +321,6 @@
     <t>REG B</t>
   </si>
   <si>
-    <t>MUX DEST</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>MUX A</t>
-  </si>
-  <si>
-    <t>MUX B</t>
-  </si>
-  <si>
     <t>IR</t>
   </si>
   <si>
@@ -394,6 +379,27 @@
   </si>
   <si>
     <t>Control</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>000001</t>
+  </si>
+  <si>
+    <t>0100</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>DEC DEST</t>
+  </si>
+  <si>
+    <t>DEC A</t>
+  </si>
+  <si>
+    <t>DEC B</t>
   </si>
 </sst>
 </file>
@@ -591,7 +597,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -628,6 +634,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -963,11 +970,543 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27995A29-5698-4805-A688-2BA7394FC415}">
+  <dimension ref="A1:F36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D45" sqref="D44:D45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>ROW()-1</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f t="shared" ref="A3:A32" si="0">ROW()-1</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" t="s">
+        <v>120</v>
+      </c>
+      <c r="E22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" t="s">
+        <v>102</v>
+      </c>
+      <c r="E31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" t="s">
+        <v>102</v>
+      </c>
+      <c r="E32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" s="12">
+        <f>COUNT(A:A)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="13"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="15">
+        <f>COUNTIF(F:F,"const 1")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="16"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" s="18">
+        <f>E34-E35</f>
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C2:C13"/>
+    <mergeCell ref="C14:C22"/>
+    <mergeCell ref="C25:C32"/>
+    <mergeCell ref="C23:C24"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="D34:D36 D16:D32 D3:D14">
+    <cfRule type="expression" priority="4">
+      <formula>$F$2="const 1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G39 G42 G17 F44:F55 E44:E1048576 E25:F37 E16:E24 F4:F19 E1:E14">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"const 1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="expression" priority="2">
+      <formula>$F$2="const 1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"const 1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F904DBB9-1FEB-4077-A5E6-86A97D866F70}">
   <dimension ref="A1:U70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1855,11 +2394,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6D5924-FD18-48E3-8129-A5F6A2CED0D8}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -1869,7 +2408,7 @@
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1886,7 +2425,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>DEC2HEX(_xlfn.NUMBERVALUE( ROW()-2),1)</f>
         <v>0</v>
@@ -1902,7 +2441,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A17" si="0">DEC2HEX(_xlfn.NUMBERVALUE( ROW()-2),1)</f>
         <v>1</v>
@@ -1918,7 +2457,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1934,7 +2473,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1950,7 +2489,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1973,7 +2512,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1996,7 +2535,7 @@
         <v>01</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2019,7 +2558,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2042,7 +2581,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2058,7 +2597,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2074,7 +2613,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -2090,7 +2629,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>B</v>
@@ -2106,7 +2645,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>C</v>
@@ -2122,7 +2661,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>D</v>
@@ -2138,7 +2677,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
@@ -2152,9 +2691,6 @@
       </c>
       <c r="D16" t="s">
         <v>14</v>
-      </c>
-      <c r="J16" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2179,12 +2715,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B656CCEA-8C5E-4FD9-9F21-21B7A6DC026C}">
-  <dimension ref="A1:V18"/>
+  <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView topLeftCell="I4" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2421,6 +2957,24 @@
         <v>57</v>
       </c>
     </row>
+    <row r="27" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>114</v>
+      </c>
+      <c r="K27" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="L27" t="str">
+        <f>HEX2BIN(0, 2)</f>
+        <v>00</v>
+      </c>
+      <c r="M27" t="s">
+        <v>116</v>
+      </c>
+      <c r="N27" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="J8:P8"/>
@@ -2433,562 +2987,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27995A29-5698-4805-A688-2BA7394FC415}">
-  <dimension ref="A1:F38"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f>ROW()-1</f>
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f t="shared" ref="A3:A34" si="0">ROW()-1</f>
-        <v>2</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D16" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" t="s">
-        <v>99</v>
-      </c>
-      <c r="E17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" t="s">
-        <v>104</v>
-      </c>
-      <c r="E19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="D20" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" t="s">
-        <v>114</v>
-      </c>
-      <c r="F20" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" t="s">
-        <v>95</v>
-      </c>
-      <c r="E22" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" t="s">
-        <v>97</v>
-      </c>
-      <c r="E23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" t="s">
-        <v>98</v>
-      </c>
-      <c r="E24" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" t="s">
-        <v>106</v>
-      </c>
-      <c r="E25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="C26" s="19"/>
-      <c r="D26" t="s">
-        <v>106</v>
-      </c>
-      <c r="E26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D27" t="s">
-        <v>93</v>
-      </c>
-      <c r="E27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="D28" t="s">
-        <v>93</v>
-      </c>
-      <c r="E28" t="s">
-        <v>88</v>
-      </c>
-      <c r="F28" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" t="s">
-        <v>100</v>
-      </c>
-      <c r="E29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="C31" s="9"/>
-      <c r="D31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E31" t="s">
-        <v>88</v>
-      </c>
-      <c r="F31" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" t="s">
-        <v>102</v>
-      </c>
-      <c r="E32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="C33" s="9"/>
-      <c r="D33" t="s">
-        <v>107</v>
-      </c>
-      <c r="E33" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="C34" s="9"/>
-      <c r="D34" t="s">
-        <v>107</v>
-      </c>
-      <c r="E34" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="E36" s="12">
-        <f>COUNT(A:A)</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="13"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="E37" s="15">
-        <f>COUNTIF(F:F,"const 1")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="16"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="E38" s="18">
-        <f>E36-E37</f>
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C2:C15"/>
-    <mergeCell ref="C16:C24"/>
-    <mergeCell ref="C27:C34"/>
-    <mergeCell ref="C25:C26"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D36:D38 D3:D16 D18:D34">
-    <cfRule type="expression" priority="4">
-      <formula>$F$2="const 1"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G41 G44 G19 E1:E16 F5:F21 F46:F57 E46:E1048576 E27:F39 E18:E26">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"const 1"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="expression" priority="2">
-      <formula>$F$2="const 1"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"const 1"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Alu add with carry + modifiers
</commit_message>
<xml_diff>
--- a/KPC8/Docs/Specs.xlsx
+++ b/KPC8/Docs/Specs.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Random\KPC8\KPC8\KPC8\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAEF8B6-7EBA-49E7-9CF8-E17C2BA980AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEDBD98-D4BB-47C8-B997-BA725F68C76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{17029D09-6E3C-4208-87C0-FA3EA582112B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{17029D09-6E3C-4208-87C0-FA3EA582112B}"/>
   </bookViews>
   <sheets>
     <sheet name="Control signals" sheetId="4" r:id="rId1"/>
     <sheet name="16BitInstructionSet" sheetId="1" r:id="rId2"/>
-    <sheet name="Interrupts" sheetId="7" r:id="rId3"/>
-    <sheet name="Registers" sheetId="2" r:id="rId4"/>
-    <sheet name="Flags" sheetId="5" r:id="rId5"/>
-    <sheet name="Instruction formats" sheetId="3" r:id="rId6"/>
+    <sheet name="ALU" sheetId="8" r:id="rId3"/>
+    <sheet name="Interrupts" sheetId="7" r:id="rId4"/>
+    <sheet name="Registers" sheetId="2" r:id="rId5"/>
+    <sheet name="Flags" sheetId="5" r:id="rId6"/>
+    <sheet name="Instruction formats" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="299">
   <si>
     <t>OPCODE HEX</t>
   </si>
@@ -215,72 +216,21 @@
     <t>Tot. Length</t>
   </si>
   <si>
-    <t>BASE ADDRESSING MODE</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
     <t>REG_DEST address:</t>
   </si>
   <si>
+    <t>nop</t>
+  </si>
+  <si>
     <t>no operation</t>
   </si>
   <si>
-    <t>set upper value of rom address register to immediate</t>
-  </si>
-  <si>
-    <t>sromau</t>
-  </si>
-  <si>
-    <t>sromal</t>
-  </si>
-  <si>
-    <t>set lower value of rom address register to immediate</t>
-  </si>
-  <si>
-    <t>sromaui</t>
-  </si>
-  <si>
-    <t>sromali</t>
-  </si>
-  <si>
-    <t>set upper value of rom address register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">set lower value of rom address register </t>
-  </si>
-  <si>
-    <t>lb</t>
-  </si>
-  <si>
-    <t>lbi</t>
-  </si>
-  <si>
     <t>load byte from ram</t>
   </si>
   <si>
-    <t>load byte from ram immediate</t>
-  </si>
-  <si>
-    <t>lb16</t>
-  </si>
-  <si>
-    <t>load byte from rom using rom address register</t>
-  </si>
-  <si>
-    <t>sb</t>
-  </si>
-  <si>
-    <t>store byte in ram</t>
-  </si>
-  <si>
-    <t>sbi</t>
-  </si>
-  <si>
-    <t>store byte in ram immediate</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -368,6 +318,9 @@
     <t>Id</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>Signal</t>
   </si>
   <si>
@@ -428,25 +381,13 @@
     <t>Flags val</t>
   </si>
   <si>
-    <t>le hi</t>
-  </si>
-  <si>
-    <t>le lo</t>
-  </si>
-  <si>
-    <t>hi</t>
-  </si>
-  <si>
-    <t>lo</t>
-  </si>
-  <si>
-    <t>hi &amp;&amp; lo</t>
-  </si>
-  <si>
-    <t>off</t>
-  </si>
-  <si>
-    <t>hilo</t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
   <si>
     <t>i</t>
@@ -485,43 +426,25 @@
     <t>jump if zero</t>
   </si>
   <si>
-    <t>nop()</t>
-  </si>
-  <si>
-    <t>jz($zero, $rCheck, $rAddress)</t>
-  </si>
-  <si>
-    <t>add($rDest, $rA, $rB)</t>
-  </si>
-  <si>
-    <t>addi($rDest, IMM8)</t>
-  </si>
-  <si>
-    <t>sub($rDest, $rA, $rB)</t>
-  </si>
-  <si>
-    <t>subi($rDest, IMM8)</t>
-  </si>
-  <si>
     <t>jge</t>
   </si>
   <si>
     <t>jl</t>
   </si>
   <si>
+    <t>jg</t>
+  </si>
+  <si>
     <t>jle</t>
   </si>
   <si>
-    <t>addc($rDest, $rA, $rB)</t>
-  </si>
-  <si>
-    <t>subc($rDest, $rA, $rB)</t>
-  </si>
-  <si>
-    <t>jn($zero, $rCheck, $rAddress)</t>
-  </si>
-  <si>
-    <t>jg($zero, $rCheck, $rAddress)</t>
+    <t>jn</t>
+  </si>
+  <si>
+    <t>addc</t>
+  </si>
+  <si>
+    <t>subc</t>
   </si>
   <si>
     <t>Code</t>
@@ -551,9 +474,6 @@
     <t>ROM Jump address</t>
   </si>
   <si>
-    <t>110100</t>
-  </si>
-  <si>
     <t>ROM INRR LO</t>
   </si>
   <si>
@@ -593,13 +513,7 @@
     <t>ROM INRR HI (interHw opcode)</t>
   </si>
   <si>
-    <t>irren($zero, IMM)</t>
-  </si>
-  <si>
-    <t>irrdis($zero, IMM)</t>
-  </si>
-  <si>
-    <t>irrex($zero, IMM)</t>
+    <t>irren</t>
   </si>
   <si>
     <t>interrupt enable</t>
@@ -611,9 +525,6 @@
     <t>Interrupts (procedural)</t>
   </si>
   <si>
-    <t>irrret($zero, IMM)</t>
-  </si>
-  <si>
     <t>return from interrupt</t>
   </si>
   <si>
@@ -669,13 +580,370 @@
   </si>
   <si>
     <t>when 1 - interrupt is pending</t>
+  </si>
+  <si>
+    <t>lbrom</t>
+  </si>
+  <si>
+    <t>lwrom</t>
+  </si>
+  <si>
+    <t>load word (2 bytes) from ram</t>
+  </si>
+  <si>
+    <t>load byte from rom</t>
+  </si>
+  <si>
+    <t>load word (2 bytes) from rom</t>
+  </si>
+  <si>
+    <t>lbram</t>
+  </si>
+  <si>
+    <t>lwram</t>
+  </si>
+  <si>
+    <t>sbram</t>
+  </si>
+  <si>
+    <t>swram</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>$rDest, $rA, $rB</t>
+  </si>
+  <si>
+    <t>addi</t>
+  </si>
+  <si>
+    <t>sub</t>
+  </si>
+  <si>
+    <t>subi</t>
+  </si>
+  <si>
+    <t>irrex</t>
+  </si>
+  <si>
+    <t>$zero, IMM</t>
+  </si>
+  <si>
+    <t>lbext</t>
+  </si>
+  <si>
+    <t>lwext</t>
+  </si>
+  <si>
+    <t>sbext</t>
+  </si>
+  <si>
+    <t>swext</t>
+  </si>
+  <si>
+    <t>irrret</t>
+  </si>
+  <si>
+    <t>irrdis</t>
+  </si>
+  <si>
+    <t>jz</t>
+  </si>
+  <si>
+    <t>$zero, $rCheck, $rAddress</t>
+  </si>
+  <si>
+    <t>Always ROM address</t>
+  </si>
+  <si>
+    <t>Always RAM address</t>
+  </si>
+  <si>
+    <t>load byte from external memory</t>
+  </si>
+  <si>
+    <t>load byte from external memory immediate</t>
+  </si>
+  <si>
+    <t>load word (2 bytes) from external memory</t>
+  </si>
+  <si>
+    <t>sbrami</t>
+  </si>
+  <si>
+    <t>sbexti</t>
+  </si>
+  <si>
+    <t>lbexti</t>
+  </si>
+  <si>
+    <t>jr</t>
+  </si>
+  <si>
+    <t>$zero, $rAddress, $rOffset</t>
+  </si>
+  <si>
+    <t>jump to address specified in $rAddress register + $rOffset</t>
+  </si>
+  <si>
+    <t>$rDest, $rAddress, $rOffset</t>
+  </si>
+  <si>
+    <t>$rDest, #value</t>
+  </si>
+  <si>
+    <t>$rDest = $rA - $rB</t>
+  </si>
+  <si>
+    <t>$rDest = $rDest + #value</t>
+  </si>
+  <si>
+    <t>$rDest = $rDest - #value</t>
+  </si>
+  <si>
+    <t>$rDest = $rA + $rB</t>
+  </si>
+  <si>
+    <t>$zero, #offset</t>
+  </si>
+  <si>
+    <t>jump to address PC + #offset</t>
+  </si>
+  <si>
+    <t>$rAddress, #offset</t>
+  </si>
+  <si>
+    <t>jump to address specified in $rAddress register + #Offset</t>
+  </si>
+  <si>
+    <t>MIXED INSTRUCTION FORMAT</t>
+  </si>
+  <si>
+    <t>$zero, $rA, $rAddress</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>$rA = *$rAddress</t>
+  </si>
+  <si>
+    <t>lbromo</t>
+  </si>
+  <si>
+    <t>load byte from rom with offset</t>
+  </si>
+  <si>
+    <t>$rDest = *($rAddress + $rOffset)</t>
+  </si>
+  <si>
+    <t>jroi</t>
+  </si>
+  <si>
+    <t>jpcoi</t>
+  </si>
+  <si>
+    <t>Full name</t>
+  </si>
+  <si>
+    <t>No operation</t>
+  </si>
+  <si>
+    <t>Load byte ROM</t>
+  </si>
+  <si>
+    <t>Load byte ROM offset</t>
+  </si>
+  <si>
+    <t>Load word ROM</t>
+  </si>
+  <si>
+    <t>Load word RAM</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Add immediate</t>
+  </si>
+  <si>
+    <t>Subtract</t>
+  </si>
+  <si>
+    <t>Subtract immediate</t>
+  </si>
+  <si>
+    <t>mov</t>
+  </si>
+  <si>
+    <t>movi</t>
+  </si>
+  <si>
+    <t>$zero, $rA, $rB</t>
+  </si>
+  <si>
+    <t>Move register</t>
+  </si>
+  <si>
+    <t>$rA = $rB</t>
+  </si>
+  <si>
+    <t>Move register immediate</t>
+  </si>
+  <si>
+    <t>$rDest = #value</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>Load byte RAM</t>
+  </si>
+  <si>
+    <t>lbramo</t>
+  </si>
+  <si>
+    <t>load byte from ram with offset</t>
+  </si>
+  <si>
+    <t>Load byte RAM offset</t>
+  </si>
+  <si>
+    <t>Store byte in RAM</t>
+  </si>
+  <si>
+    <t>Store byte in RAM immediate</t>
+  </si>
+  <si>
+    <t>Store word in RAM</t>
+  </si>
+  <si>
+    <t>pushb</t>
+  </si>
+  <si>
+    <t>pushw</t>
+  </si>
+  <si>
+    <t>popb</t>
+  </si>
+  <si>
+    <t>popw</t>
+  </si>
+  <si>
+    <t>Push byte</t>
+  </si>
+  <si>
+    <t>Push word</t>
+  </si>
+  <si>
+    <t>Pop byte</t>
+  </si>
+  <si>
+    <t>Pop word</t>
+  </si>
+  <si>
+    <t>load byte from RAM and decrement address by 1</t>
+  </si>
+  <si>
+    <t>load word from RAM and decrement address by 2</t>
+  </si>
+  <si>
+    <t>store byte in RAM and increment address by 1</t>
+  </si>
+  <si>
+    <t>store byte in RAM and increment address by 2</t>
+  </si>
+  <si>
+    <t>*$rAddress = $rA; $rAddress += 1</t>
+  </si>
+  <si>
+    <t>*$rAddress = $rA; $rAddress += 2</t>
+  </si>
+  <si>
+    <t>$rA = *$rAddress; $rAddress -= 1</t>
+  </si>
+  <si>
+    <t>$rA = *$rAddress; $rAddress -= 2</t>
+  </si>
+  <si>
+    <t>Offset value in range [0, 255]</t>
+  </si>
+  <si>
+    <t>subtract</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>xor</t>
+  </si>
+  <si>
+    <t>sl</t>
+  </si>
+  <si>
+    <t>sr</t>
+  </si>
+  <si>
+    <t>Primary operation</t>
+  </si>
+  <si>
+    <t>Secondary operation</t>
+  </si>
+  <si>
+    <t>add 16 bit (2x8 bit, hi with carry)</t>
+  </si>
+  <si>
+    <t>subtract 16 bit (2x8 bit, hi with carry)</t>
+  </si>
+  <si>
+    <t>sll</t>
+  </si>
+  <si>
+    <t>srl</t>
+  </si>
+  <si>
+    <t>Shift right logical</t>
+  </si>
+  <si>
+    <t>Shift left logical</t>
+  </si>
+  <si>
+    <t>Bitwise AND</t>
+  </si>
+  <si>
+    <t>Bitwise XOR</t>
+  </si>
+  <si>
+    <t>Bitwise OR</t>
+  </si>
+  <si>
+    <t>Bitwise NOT</t>
+  </si>
+  <si>
+    <t>subtract 8 bit, no carry</t>
+  </si>
+  <si>
+    <t>Add with carry</t>
+  </si>
+  <si>
+    <t>Subtract with carry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -709,6 +977,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -724,7 +1000,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -734,6 +1010,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -930,19 +1211,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -952,17 +1237,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -974,26 +1260,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1005,21 +1291,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="4" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
-    <cellStyle name="20% - Accent2" xfId="5" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
-    <cellStyle name="60% - Accent3" xfId="7" builtinId="40"/>
+  <cellStyles count="9">
+    <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
+    <cellStyle name="20% - Accent2" xfId="6" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="7" builtinId="35"/>
+    <cellStyle name="60% - Accent3" xfId="8" builtinId="40"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Input" xfId="3" builtinId="20"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="Input" xfId="4" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1365,23 +1664,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>59</v>
+      <c r="D1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1389,14 +1688,14 @@
         <f>ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>110</v>
+      <c r="C2" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1404,12 +1703,12 @@
         <f t="shared" ref="A3:A32" si="0">ROW()-1</f>
         <v>2</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1417,12 +1716,12 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="9"/>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1430,12 +1729,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="9"/>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1443,12 +1742,12 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="9"/>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1456,12 +1755,12 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="9"/>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1469,15 +1768,15 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="9"/>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="E8" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="F8" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1485,12 +1784,12 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="9"/>
       <c r="D9" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1498,12 +1797,12 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="9"/>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1511,12 +1810,12 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="9"/>
       <c r="D11" t="s">
         <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1524,12 +1823,12 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="9"/>
       <c r="D12" t="s">
         <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1537,12 +1836,12 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="9"/>
       <c r="D13" t="s">
         <v>47</v>
       </c>
       <c r="E13" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1550,14 +1849,14 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>111</v>
+      <c r="C14" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1565,12 +1864,12 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C15" s="8"/>
+      <c r="C15" s="10"/>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1578,15 +1877,15 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C16" s="8"/>
+      <c r="C16" s="10"/>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="F16" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1594,12 +1893,12 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="10"/>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="E17" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1607,15 +1906,15 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="C18" s="10"/>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="F18" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1623,12 +1922,12 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C19" s="8"/>
+      <c r="C19" s="10"/>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="E19" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1636,12 +1935,12 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C20" s="8"/>
+      <c r="C20" s="10"/>
       <c r="D20" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="E20" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1649,12 +1948,12 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C21" s="8"/>
+      <c r="C21" s="10"/>
       <c r="D21" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1662,12 +1961,12 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C22" s="8"/>
+      <c r="C22" s="10"/>
       <c r="D22" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1675,14 +1974,14 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>99</v>
+      <c r="C23" s="21" t="s">
+        <v>82</v>
       </c>
       <c r="D23" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1690,12 +1989,12 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C24" s="19"/>
+      <c r="C24" s="21"/>
       <c r="D24" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E24" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1703,14 +2002,14 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>100</v>
+      <c r="C25" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E25" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1718,15 +2017,15 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C26" s="9"/>
+      <c r="C26" s="11"/>
       <c r="D26" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E26" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="F26" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1734,12 +2033,12 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C27" s="9"/>
+      <c r="C27" s="11"/>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1747,12 +2046,12 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="C28" s="9"/>
+      <c r="C28" s="11"/>
       <c r="D28" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="E28" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1760,15 +2059,15 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C29" s="9"/>
+      <c r="C29" s="11"/>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="E29" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="F29" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1776,12 +2075,12 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="C30" s="9"/>
+      <c r="C30" s="11"/>
       <c r="D30" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="E30" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1789,12 +2088,12 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="C31" s="9"/>
+      <c r="C31" s="11"/>
       <c r="D31" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="E31" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1802,46 +2101,46 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="C32" s="9"/>
+      <c r="C32" s="11"/>
       <c r="D32" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="E32" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E34" s="12">
+      <c r="B34" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" s="14">
         <f>COUNT(A:A)</f>
         <v>31</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="13"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="E35" s="15">
+      <c r="B35" s="15"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" s="17">
         <f>COUNTIF(F:F,"const 1")</f>
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="16"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="E36" s="18">
+      <c r="B36" s="18"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="20">
         <f>E34-E35</f>
         <v>26</v>
       </c>
@@ -1881,10 +2180,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F904DBB9-1FEB-4077-A5E6-86A97D866F70}">
-  <dimension ref="A1:V70"/>
+  <dimension ref="A1:W70"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1893,911 +2192,1245 @@
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" style="3" customWidth="1"/>
-    <col min="18" max="18" width="17.140625" customWidth="1"/>
-    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.28515625" customWidth="1"/>
-    <col min="22" max="22" width="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="30" style="4" customWidth="1"/>
+    <col min="7" max="7" width="53" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.28515625" customWidth="1"/>
+    <col min="9" max="9" width="31.5703125" customWidth="1"/>
+    <col min="19" max="19" width="17.140625" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.28515625" customWidth="1"/>
+    <col min="23" max="23" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="V1" t="s">
+      <c r="H1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="W1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
         <f>DEC2HEX(_xlfn.NUMBERVALUE( ROW()-2),2)</f>
         <v>00</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>124</v>
+      <c r="B2" s="23" t="s">
+        <v>108</v>
       </c>
       <c r="C2" t="str">
         <f>HEX2BIN(A2,6)</f>
         <v>000000</v>
       </c>
-      <c r="D2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:A65" si="0">DEC2HEX(_xlfn.NUMBERVALUE( ROW()-2),2)</f>
         <v>01</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="23"/>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C65" si="1">HEX2BIN(A3,6)</f>
         <v>000001</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="V3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="H3" t="s">
+        <v>230</v>
+      </c>
+      <c r="W3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>02</v>
       </c>
-      <c r="B4" s="21"/>
+      <c r="B4" s="23"/>
       <c r="C4" t="str">
         <f t="shared" si="1"/>
         <v>000010</v>
       </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="V4" t="s">
+      <c r="D4" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="H4" t="s">
+        <v>233</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="W4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>03</v>
       </c>
-      <c r="B5" s="21"/>
+      <c r="B5" s="23"/>
       <c r="C5" t="str">
         <f t="shared" si="1"/>
         <v>000011</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="H5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>04</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="23"/>
       <c r="C6" t="str">
         <f t="shared" si="1"/>
         <v>000100</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>05</v>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="23"/>
       <c r="C7" t="str">
         <f t="shared" si="1"/>
         <v>000101</v>
       </c>
-      <c r="D7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>06</v>
       </c>
-      <c r="B8" s="21"/>
+      <c r="B8" s="23"/>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
         <v>000110</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>07</v>
       </c>
-      <c r="B9" s="21"/>
+      <c r="B9" s="23"/>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
         <v>000111</v>
       </c>
-      <c r="D9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D9" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>08</v>
       </c>
-      <c r="B10" s="21"/>
+      <c r="B10" s="23"/>
       <c r="C10" t="str">
         <f t="shared" si="1"/>
         <v>001000</v>
       </c>
-      <c r="D10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D10" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>09</v>
       </c>
-      <c r="B11" s="21"/>
+      <c r="B11" s="23"/>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
         <v>001001</v>
       </c>
-      <c r="D11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D11" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0A</v>
       </c>
-      <c r="B12" s="21"/>
+      <c r="B12" s="23"/>
       <c r="C12" t="str">
         <f t="shared" si="1"/>
         <v>001010</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0B</v>
       </c>
-      <c r="B13" s="21"/>
+      <c r="B13" s="23"/>
       <c r="C13" t="str">
         <f t="shared" si="1"/>
         <v>001011</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>211</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0C</v>
       </c>
-      <c r="B14" s="21"/>
+      <c r="B14" s="23"/>
       <c r="C14" t="str">
         <f t="shared" si="1"/>
         <v>001100</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>188</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0D</v>
       </c>
-      <c r="B15" s="21"/>
+      <c r="B15" s="23"/>
       <c r="C15" t="str">
         <f t="shared" si="1"/>
         <v>001101</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D15" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0E</v>
       </c>
-      <c r="B16" s="21"/>
+      <c r="B16" s="23"/>
       <c r="C16" t="str">
         <f t="shared" si="1"/>
         <v>001110</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>0F</v>
       </c>
-      <c r="B17" s="21"/>
+      <c r="B17" s="23"/>
       <c r="C17" t="str">
         <f t="shared" si="1"/>
         <v>001111</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B18" s="21"/>
+      <c r="B18" s="23"/>
       <c r="C18" t="str">
         <f t="shared" si="1"/>
         <v>010000</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="H18" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>010001</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="H19" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B20" s="23"/>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v>010010</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="G20" t="s">
+        <v>296</v>
+      </c>
+      <c r="H20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>010011</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="G21" t="s">
+        <v>296</v>
+      </c>
+      <c r="H21" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" t="str">
+        <f t="shared" si="1"/>
+        <v>010100</v>
+      </c>
+      <c r="D22" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="G22" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B23" s="23"/>
+      <c r="C23" t="str">
+        <f t="shared" si="1"/>
+        <v>010101</v>
+      </c>
+      <c r="D23" t="s">
+        <v>134</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="G23" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B24" s="23"/>
+      <c r="C24" t="str">
+        <f t="shared" si="1"/>
+        <v>010110</v>
+      </c>
+      <c r="D24" t="s">
+        <v>280</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B25" s="23"/>
+      <c r="C25" t="str">
+        <f t="shared" si="1"/>
+        <v>010111</v>
+      </c>
+      <c r="D25" t="s">
+        <v>254</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B26" s="23"/>
+      <c r="C26" t="str">
+        <f t="shared" si="1"/>
+        <v>011000</v>
+      </c>
+      <c r="D26" t="s">
+        <v>253</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" t="str">
+        <f t="shared" si="1"/>
+        <v>011001</v>
+      </c>
+      <c r="D27" t="s">
+        <v>281</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1A</v>
+      </c>
+      <c r="B28" s="23"/>
+      <c r="C28" t="str">
+        <f t="shared" si="1"/>
+        <v>011010</v>
+      </c>
+      <c r="D28" t="s">
+        <v>288</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1B</v>
+      </c>
+      <c r="B29" s="23"/>
+      <c r="C29" t="str">
+        <f t="shared" si="1"/>
+        <v>011011</v>
+      </c>
+      <c r="D29" t="s">
+        <v>289</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1C</v>
+      </c>
+      <c r="B30" s="23"/>
+      <c r="C30" t="str">
+        <f t="shared" si="1"/>
+        <v>011100</v>
+      </c>
+      <c r="D30" t="s">
+        <v>214</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1D</v>
+      </c>
+      <c r="B31" s="23"/>
+      <c r="C31" t="str">
+        <f t="shared" si="1"/>
+        <v>011101</v>
+      </c>
+      <c r="D31" t="s">
+        <v>234</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="G31" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1E</v>
+      </c>
+      <c r="B32" s="23"/>
+      <c r="C32" t="str">
+        <f t="shared" si="1"/>
+        <v>011110</v>
+      </c>
+      <c r="D32" t="s">
+        <v>235</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G32" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1F</v>
+      </c>
+      <c r="B33" s="23"/>
+      <c r="C33" t="str">
+        <f t="shared" si="1"/>
+        <v>011111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B34" s="23"/>
+      <c r="C34" t="str">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="G34" t="s">
+        <v>270</v>
+      </c>
+      <c r="H34" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B35" s="23"/>
+      <c r="C35" t="str">
+        <f t="shared" si="1"/>
+        <v>100001</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="G35" t="s">
+        <v>271</v>
+      </c>
+      <c r="H35" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B36" s="23"/>
+      <c r="C36" t="str">
+        <f t="shared" si="1"/>
+        <v>100010</v>
+      </c>
+      <c r="D36" s="36" t="s">
+        <v>262</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="G36" t="s">
+        <v>272</v>
+      </c>
+      <c r="H36" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B37" s="23"/>
+      <c r="C37" t="str">
+        <f t="shared" si="1"/>
+        <v>100011</v>
+      </c>
+      <c r="D37" s="36" t="s">
+        <v>263</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="G37" t="s">
+        <v>273</v>
+      </c>
+      <c r="H37" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B38" s="23"/>
+      <c r="C38" t="str">
+        <f t="shared" si="1"/>
+        <v>100100</v>
+      </c>
+      <c r="D38" t="s">
+        <v>246</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="H38" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B39" s="23"/>
+      <c r="C39" t="str">
+        <f t="shared" si="1"/>
+        <v>100101</v>
+      </c>
+      <c r="D39" t="s">
+        <v>247</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="H39" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B40" s="23"/>
+      <c r="C40" t="str">
+        <f t="shared" si="1"/>
+        <v>100110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B41" s="23"/>
+      <c r="C41" t="str">
+        <f t="shared" si="1"/>
+        <v>100111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B42" s="23"/>
+      <c r="C42" t="str">
+        <f t="shared" si="1"/>
+        <v>101000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B43" s="23"/>
+      <c r="C43" t="str">
+        <f t="shared" si="1"/>
+        <v>101001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2A</v>
+      </c>
+      <c r="B44" s="23"/>
+      <c r="C44" t="str">
+        <f t="shared" si="1"/>
+        <v>101010</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2B</v>
+      </c>
+      <c r="B45" s="23"/>
+      <c r="C45" t="str">
+        <f t="shared" si="1"/>
+        <v>101011</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2C</v>
+      </c>
+      <c r="B46" s="23"/>
+      <c r="C46" t="str">
+        <f t="shared" si="1"/>
+        <v>101100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2D</v>
+      </c>
+      <c r="B47" s="23"/>
+      <c r="C47" t="str">
+        <f t="shared" si="1"/>
+        <v>101101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2E</v>
+      </c>
+      <c r="B48" s="23"/>
+      <c r="C48" t="str">
+        <f t="shared" si="1"/>
+        <v>101110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2F</v>
+      </c>
+      <c r="B49" s="23"/>
+      <c r="C49" t="str">
+        <f t="shared" si="1"/>
+        <v>101111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B50" s="23"/>
+      <c r="C50" t="str">
+        <f t="shared" si="1"/>
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B51" s="23"/>
+      <c r="C51" t="str">
+        <f t="shared" si="1"/>
+        <v>110001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B52" s="23"/>
+      <c r="C52" t="str">
+        <f t="shared" si="1"/>
+        <v>110010</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B53" s="25"/>
+      <c r="C53" t="str">
+        <f t="shared" si="1"/>
+        <v>110011</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="1"/>
+        <v>110100</v>
+      </c>
+      <c r="D54" t="s">
+        <v>196</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B55" s="27"/>
+      <c r="C55" t="str">
+        <f t="shared" si="1"/>
+        <v>110101</v>
+      </c>
+      <c r="D55" t="s">
+        <v>202</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B56" s="27"/>
+      <c r="C56" t="str">
+        <f t="shared" si="1"/>
+        <v>110110</v>
+      </c>
+      <c r="D56" t="s">
+        <v>157</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B57" s="28"/>
+      <c r="C57" t="str">
+        <f t="shared" si="1"/>
+        <v>110111</v>
+      </c>
+      <c r="D57" t="s">
+        <v>203</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B58" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="1"/>
+        <v>111000</v>
+      </c>
+      <c r="D58" t="s">
+        <v>204</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B59" s="24"/>
+      <c r="C59" t="str">
+        <f t="shared" si="1"/>
+        <v>111001</v>
+      </c>
+      <c r="D59" t="s">
+        <v>132</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3A</v>
+      </c>
+      <c r="B60" s="24"/>
+      <c r="C60" t="str">
+        <f t="shared" si="1"/>
+        <v>111010</v>
+      </c>
+      <c r="D60" t="s">
+        <v>130</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3B</v>
+      </c>
+      <c r="B61" s="24"/>
+      <c r="C61" t="str">
+        <f t="shared" si="1"/>
+        <v>111011</v>
+      </c>
+      <c r="D61" t="s">
+        <v>128</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3C</v>
+      </c>
+      <c r="B62" s="24"/>
+      <c r="C62" t="str">
+        <f t="shared" si="1"/>
+        <v>111100</v>
+      </c>
+      <c r="D62" t="s">
+        <v>129</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3D</v>
+      </c>
+      <c r="B63" s="24"/>
+      <c r="C63" t="str">
+        <f t="shared" si="1"/>
+        <v>111101</v>
+      </c>
+      <c r="D63" t="s">
+        <v>131</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3E</v>
+      </c>
+      <c r="B64" s="24"/>
+      <c r="C64" t="str">
+        <f t="shared" si="1"/>
+        <v>111110</v>
+      </c>
+      <c r="D64" t="s">
+        <v>133</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G64" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" t="str">
-        <f t="shared" si="1"/>
-        <v>010001</v>
-      </c>
-      <c r="D19" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3F</v>
+      </c>
+      <c r="B65" s="24"/>
+      <c r="C65" t="str">
+        <f t="shared" si="1"/>
+        <v>111111</v>
+      </c>
+      <c r="D65" t="s">
+        <v>134</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G65" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B20" s="21"/>
-      <c r="C20" t="str">
-        <f t="shared" si="1"/>
-        <v>010010</v>
-      </c>
-      <c r="D20" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B21" s="21"/>
-      <c r="C21" t="str">
-        <f t="shared" si="1"/>
-        <v>010011</v>
-      </c>
-      <c r="D21" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B22" s="21"/>
-      <c r="C22" t="str">
-        <f t="shared" si="1"/>
-        <v>010100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B23" s="21"/>
-      <c r="C23" t="str">
-        <f t="shared" si="1"/>
-        <v>010101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B24" s="21"/>
-      <c r="C24" t="str">
-        <f t="shared" si="1"/>
-        <v>010110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B25" s="21"/>
-      <c r="C25" t="str">
-        <f t="shared" si="1"/>
-        <v>010111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B26" s="21"/>
-      <c r="C26" t="str">
-        <f t="shared" si="1"/>
-        <v>011000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B27" s="21"/>
-      <c r="C27" t="str">
-        <f t="shared" si="1"/>
-        <v>011001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>1A</v>
-      </c>
-      <c r="B28" s="21"/>
-      <c r="C28" t="str">
-        <f t="shared" si="1"/>
-        <v>011010</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>1B</v>
-      </c>
-      <c r="B29" s="21"/>
-      <c r="C29" t="str">
-        <f t="shared" si="1"/>
-        <v>011011</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>1C</v>
-      </c>
-      <c r="B30" s="21"/>
-      <c r="C30" t="str">
-        <f t="shared" si="1"/>
-        <v>011100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>1D</v>
-      </c>
-      <c r="B31" s="21"/>
-      <c r="C31" t="str">
-        <f t="shared" si="1"/>
-        <v>011101</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>1E</v>
-      </c>
-      <c r="B32" s="21"/>
-      <c r="C32" t="str">
-        <f t="shared" si="1"/>
-        <v>011110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>1F</v>
-      </c>
-      <c r="B33" s="21"/>
-      <c r="C33" t="str">
-        <f t="shared" si="1"/>
-        <v>011111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B34" s="21"/>
-      <c r="C34" t="str">
-        <f t="shared" si="1"/>
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B35" s="21"/>
-      <c r="C35" t="str">
-        <f t="shared" si="1"/>
-        <v>100001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B36" s="21"/>
-      <c r="C36" t="str">
-        <f t="shared" si="1"/>
-        <v>100010</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B37" s="21"/>
-      <c r="C37" t="str">
-        <f t="shared" si="1"/>
-        <v>100011</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B38" s="21"/>
-      <c r="C38" t="str">
-        <f t="shared" si="1"/>
-        <v>100100</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B39" s="21"/>
-      <c r="C39" t="str">
-        <f t="shared" si="1"/>
-        <v>100101</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B40" s="21"/>
-      <c r="C40" t="str">
-        <f t="shared" si="1"/>
-        <v>100110</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B41" s="21"/>
-      <c r="C41" t="str">
-        <f t="shared" si="1"/>
-        <v>100111</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B42" s="21"/>
-      <c r="C42" t="str">
-        <f t="shared" si="1"/>
-        <v>101000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B43" s="21"/>
-      <c r="C43" t="str">
-        <f t="shared" si="1"/>
-        <v>101001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>2A</v>
-      </c>
-      <c r="B44" s="21"/>
-      <c r="C44" t="str">
-        <f t="shared" si="1"/>
-        <v>101010</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>2B</v>
-      </c>
-      <c r="B45" s="21"/>
-      <c r="C45" t="str">
-        <f t="shared" si="1"/>
-        <v>101011</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>2C</v>
-      </c>
-      <c r="B46" s="21"/>
-      <c r="C46" t="str">
-        <f t="shared" si="1"/>
-        <v>101100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>2D</v>
-      </c>
-      <c r="B47" s="21"/>
-      <c r="C47" t="str">
-        <f t="shared" si="1"/>
-        <v>101101</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>2E</v>
-      </c>
-      <c r="B48" s="21"/>
-      <c r="C48" t="str">
-        <f t="shared" si="1"/>
-        <v>101110</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>2F</v>
-      </c>
-      <c r="B49" s="21"/>
-      <c r="C49" t="str">
-        <f t="shared" si="1"/>
-        <v>101111</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B50" s="21"/>
-      <c r="C50" t="str">
-        <f t="shared" si="1"/>
-        <v>110000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B51" s="21"/>
-      <c r="C51" t="str">
-        <f t="shared" si="1"/>
-        <v>110001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B52" s="21"/>
-      <c r="C52" t="str">
-        <f t="shared" si="1"/>
-        <v>110010</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B53" s="23"/>
-      <c r="C53" t="str">
-        <f t="shared" si="1"/>
-        <v>110011</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B54" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="C54" t="str">
-        <f t="shared" si="1"/>
-        <v>110100</v>
-      </c>
-      <c r="D54" t="s">
-        <v>186</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="B55" s="25"/>
-      <c r="C55" t="str">
-        <f t="shared" si="1"/>
-        <v>110101</v>
-      </c>
-      <c r="D55" t="s">
-        <v>190</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="B56" s="25"/>
-      <c r="C56" t="str">
-        <f t="shared" si="1"/>
-        <v>110110</v>
-      </c>
-      <c r="D56" t="s">
-        <v>184</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="B57" s="26"/>
-      <c r="C57" t="str">
-        <f t="shared" si="1"/>
-        <v>110111</v>
-      </c>
-      <c r="D57" t="s">
-        <v>185</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="B58" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="C58" t="str">
-        <f t="shared" si="1"/>
-        <v>111000</v>
-      </c>
-      <c r="D58" t="s">
-        <v>149</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="B59" s="22"/>
-      <c r="C59" t="str">
-        <f t="shared" si="1"/>
-        <v>111001</v>
-      </c>
-      <c r="D59" t="s">
-        <v>159</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3A</v>
-      </c>
-      <c r="B60" s="22"/>
-      <c r="C60" t="str">
-        <f t="shared" si="1"/>
-        <v>111010</v>
-      </c>
-      <c r="D60" t="s">
-        <v>160</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3B</v>
-      </c>
-      <c r="B61" s="22"/>
-      <c r="C61" t="str">
-        <f t="shared" si="1"/>
-        <v>111011</v>
-      </c>
-      <c r="D61" t="s">
-        <v>154</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3C</v>
-      </c>
-      <c r="B62" s="22"/>
-      <c r="C62" t="str">
-        <f t="shared" si="1"/>
-        <v>111100</v>
-      </c>
-      <c r="D62" t="s">
-        <v>155</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3D</v>
-      </c>
-      <c r="B63" s="22"/>
-      <c r="C63" t="str">
-        <f t="shared" si="1"/>
-        <v>111101</v>
-      </c>
-      <c r="D63" t="s">
-        <v>156</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3E</v>
-      </c>
-      <c r="B64" s="22"/>
-      <c r="C64" t="str">
-        <f t="shared" si="1"/>
-        <v>111110</v>
-      </c>
-      <c r="D64" t="s">
-        <v>157</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3F</v>
-      </c>
-      <c r="B65" s="22"/>
-      <c r="C65" t="str">
-        <f t="shared" si="1"/>
-        <v>111111</v>
-      </c>
-      <c r="D65" t="s">
-        <v>158</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
     </row>
@@ -2807,17 +3440,190 @@
     <mergeCell ref="B54:B57"/>
     <mergeCell ref="B2:B53"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE01AAB-30CE-42AF-B339-E98C8A407AFE}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="E3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="E4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="E8" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="E9" t="s">
+        <v>283</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6777839-035A-4695-B7B0-93449B7EEA83}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2833,30 +3639,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>183</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
+      <c r="A1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
@@ -2871,8 +3677,8 @@
         <f>DEC2HEX(HEX2DEC("ffff")+1-2*8*(1+HEX2DEC(A2)))</f>
         <v>FFF0</v>
       </c>
-      <c r="D2" t="s">
-        <v>170</v>
+      <c r="D2">
+        <v>11010000</v>
       </c>
       <c r="E2" t="str">
         <f>HEX2BIN(RIGHT(C2,2),8)</f>
@@ -2882,19 +3688,19 @@
         <v>55</v>
       </c>
       <c r="J2" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
       <c r="K2" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="L2" t="s">
-        <v>202</v>
+        <v>172</v>
       </c>
       <c r="M2" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="N2" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="P2" t="s">
         <v>57</v>
@@ -2913,8 +3719,8 @@
         <f t="shared" ref="C3:C17" si="2">DEC2HEX(HEX2DEC("ffff")+1-2*8*(1+HEX2DEC(A3)))</f>
         <v>FFE0</v>
       </c>
-      <c r="D3" t="s">
-        <v>170</v>
+      <c r="D3">
+        <v>11010000</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E17" si="3">HEX2BIN(RIGHT(C3,2),8)</f>
@@ -2939,7 +3745,7 @@
         <v>4</v>
       </c>
       <c r="P3" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -2955,8 +3761,8 @@
         <f t="shared" si="2"/>
         <v>FFD0</v>
       </c>
-      <c r="D4" t="s">
-        <v>170</v>
+      <c r="D4">
+        <v>11010000</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="3"/>
@@ -2976,27 +3782,27 @@
         <f t="shared" si="2"/>
         <v>FFC0</v>
       </c>
-      <c r="D5" t="s">
-        <v>170</v>
+      <c r="D5">
+        <v>11010000</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="3"/>
         <v>11000000</v>
       </c>
       <c r="J5" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="K5" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="L5" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="M5" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="N5" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="75" x14ac:dyDescent="0.25">
@@ -3012,27 +3818,27 @@
         <f t="shared" si="2"/>
         <v>FFB0</v>
       </c>
-      <c r="D6" t="s">
-        <v>170</v>
+      <c r="D6">
+        <v>11010000</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="3"/>
         <v>10110000</v>
       </c>
-      <c r="J6" s="29" t="s">
-        <v>209</v>
-      </c>
-      <c r="K6" s="27" t="s">
-        <v>204</v>
-      </c>
-      <c r="L6" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="M6" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="N6" s="27" t="s">
-        <v>166</v>
+      <c r="J6" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="K6" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="L6" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="M6" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="N6" s="29" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -3048,18 +3854,18 @@
         <f t="shared" si="2"/>
         <v>FFA0</v>
       </c>
-      <c r="D7" t="s">
-        <v>170</v>
+      <c r="D7">
+        <v>11010000</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="3"/>
         <v>10100000</v>
       </c>
-      <c r="K7" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="L7" s="29" t="s">
-        <v>180</v>
+      <c r="K7" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="L7" s="31" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -3075,24 +3881,24 @@
         <f t="shared" si="2"/>
         <v>FF90</v>
       </c>
-      <c r="D8" t="s">
-        <v>170</v>
+      <c r="D8">
+        <v>11010000</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="3"/>
         <v>10010000</v>
       </c>
       <c r="J8" t="s">
-        <v>179</v>
-      </c>
-      <c r="K8" s="28" t="s">
-        <v>205</v>
-      </c>
-      <c r="L8" s="28" t="s">
-        <v>205</v>
-      </c>
-      <c r="M8" s="28" t="s">
-        <v>205</v>
+        <v>152</v>
+      </c>
+      <c r="K8" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="L8" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="M8" s="30" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -3108,8 +3914,8 @@
         <f t="shared" si="2"/>
         <v>FF80</v>
       </c>
-      <c r="D9" t="s">
-        <v>170</v>
+      <c r="D9">
+        <v>11010000</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="3"/>
@@ -3129,8 +3935,8 @@
         <f t="shared" si="2"/>
         <v>FF70</v>
       </c>
-      <c r="D10" t="s">
-        <v>170</v>
+      <c r="D10">
+        <v>11010000</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="3"/>
@@ -3150,8 +3956,8 @@
         <f t="shared" si="2"/>
         <v>FF60</v>
       </c>
-      <c r="D11" t="s">
-        <v>170</v>
+      <c r="D11">
+        <v>11010000</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="3"/>
@@ -3171,8 +3977,8 @@
         <f t="shared" si="2"/>
         <v>FF50</v>
       </c>
-      <c r="D12" t="s">
-        <v>170</v>
+      <c r="D12">
+        <v>11010000</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="3"/>
@@ -3192,8 +3998,8 @@
         <f t="shared" si="2"/>
         <v>FF40</v>
       </c>
-      <c r="D13" t="s">
-        <v>170</v>
+      <c r="D13">
+        <v>11010000</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="3"/>
@@ -3213,8 +4019,8 @@
         <f t="shared" si="2"/>
         <v>FF30</v>
       </c>
-      <c r="D14" t="s">
-        <v>170</v>
+      <c r="D14">
+        <v>11010000</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="3"/>
@@ -3234,8 +4040,8 @@
         <f t="shared" si="2"/>
         <v>FF20</v>
       </c>
-      <c r="D15" t="s">
-        <v>170</v>
+      <c r="D15">
+        <v>11010000</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="3"/>
@@ -3255,18 +4061,18 @@
         <f t="shared" si="2"/>
         <v>FF10</v>
       </c>
-      <c r="D16" t="s">
-        <v>170</v>
+      <c r="D16">
+        <v>11010000</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="3"/>
         <v>00010000</v>
       </c>
-      <c r="J16" s="30" t="s">
-        <v>207</v>
-      </c>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
+      <c r="J16" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
@@ -3281,21 +4087,21 @@
         <f t="shared" si="2"/>
         <v>FF00</v>
       </c>
-      <c r="D17" t="s">
-        <v>170</v>
+      <c r="D17">
+        <v>11010000</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
       <c r="J17" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
       <c r="K17" t="s">
-        <v>195</v>
+        <v>165</v>
       </c>
       <c r="L17" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -3306,7 +4112,7 @@
         <v>0</v>
       </c>
       <c r="L18" t="s">
-        <v>197</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -3317,7 +4123,7 @@
         <v>1</v>
       </c>
       <c r="L19" t="s">
-        <v>198</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -3328,7 +4134,7 @@
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -3339,7 +4145,7 @@
         <v>1</v>
       </c>
       <c r="L21" t="s">
-        <v>200</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3353,12 +4159,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6D5924-FD18-48E3-8129-A5F6A2CED0D8}">
-  <dimension ref="A1:AB31"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="N18" sqref="N17:O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3367,24 +4173,52 @@
     <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="I1" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>DEC2HEX(_xlfn.NUMBERVALUE( ROW()-2),1)</f>
         <v>0</v>
@@ -3399,8 +4233,25 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A17" si="0">DEC2HEX(_xlfn.NUMBERVALUE( ROW()-2),1)</f>
         <v>1</v>
@@ -3415,8 +4266,20 @@
       <c r="D3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -3431,8 +4294,23 @@
       <c r="D4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>207</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3447,8 +4325,23 @@
       <c r="D5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>207</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3464,14 +4357,26 @@
         <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" t="str">
         <f>RIGHT(B6,2)</f>
         <v>00</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3487,14 +4392,26 @@
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" ref="F7:F9" si="2">RIGHT(B7,2)</f>
         <v>01</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3510,14 +4427,26 @@
         <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3533,14 +4462,31 @@
         <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3555,35 +4501,8 @@
       <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="S10" t="s">
-        <v>136</v>
-      </c>
-      <c r="T10" t="s">
-        <v>137</v>
-      </c>
-      <c r="U10" t="s">
-        <v>138</v>
-      </c>
-      <c r="W10" t="s">
-        <v>139</v>
-      </c>
-      <c r="X10" t="s">
-        <v>140</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>141</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>142</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3598,31 +4517,8 @@
       <c r="D11" t="s">
         <v>34</v>
       </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>134</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-      <c r="W11" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="4"/>
-      <c r="Z11" s="4"/>
-      <c r="AA11" s="4"/>
-      <c r="AB11" s="4"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -3637,26 +4533,8 @@
       <c r="D12" t="s">
         <v>35</v>
       </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>131</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>1</v>
-      </c>
-      <c r="AB12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>B</v>
@@ -3671,26 +4549,8 @@
       <c r="D13" t="s">
         <v>26</v>
       </c>
-      <c r="P13">
-        <v>2</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>132</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <v>1</v>
-      </c>
-      <c r="U13">
-        <v>0</v>
-      </c>
-      <c r="Z13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>C</v>
@@ -3705,35 +4565,8 @@
       <c r="D14" t="s">
         <v>27</v>
       </c>
-      <c r="K14" t="s">
-        <v>129</v>
-      </c>
-      <c r="L14" t="s">
-        <v>131</v>
-      </c>
-      <c r="N14" t="s">
-        <v>133</v>
-      </c>
-      <c r="P14">
-        <v>3</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>135</v>
-      </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <v>1</v>
-      </c>
-      <c r="U14">
-        <v>1</v>
-      </c>
-      <c r="Y14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>D</v>
@@ -3748,26 +4581,8 @@
       <c r="D15" t="s">
         <v>28</v>
       </c>
-      <c r="K15" t="s">
-        <v>130</v>
-      </c>
-      <c r="L15" t="s">
-        <v>132</v>
-      </c>
-      <c r="S15">
-        <v>1</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-      <c r="U15">
-        <v>0</v>
-      </c>
-      <c r="X15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
@@ -3782,20 +4597,8 @@
       <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="S16">
-        <v>1</v>
-      </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <v>1</v>
-      </c>
-      <c r="W16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
@@ -3810,156 +4613,29 @@
       <c r="D17" t="s">
         <v>38</v>
       </c>
-      <c r="S17">
-        <v>1</v>
-      </c>
-      <c r="T17">
-        <v>1</v>
-      </c>
-      <c r="U17">
-        <v>0</v>
-      </c>
-      <c r="AA17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S18">
-        <v>1</v>
-      </c>
-      <c r="T18">
-        <v>1</v>
-      </c>
-      <c r="U18">
-        <v>1</v>
-      </c>
-      <c r="W18" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
-      <c r="AA18" s="4"/>
-      <c r="AB18" s="4"/>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S23" t="s">
-        <v>136</v>
-      </c>
-      <c r="T23" t="s">
-        <v>137</v>
-      </c>
-      <c r="U23" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S24">
-        <v>0</v>
-      </c>
-      <c r="T24">
-        <v>0</v>
-      </c>
-      <c r="U24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S25">
-        <v>0</v>
-      </c>
-      <c r="T25">
-        <v>0</v>
-      </c>
-      <c r="U25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S26">
-        <v>0</v>
-      </c>
-      <c r="T26">
-        <v>1</v>
-      </c>
-      <c r="U26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S27">
-        <v>0</v>
-      </c>
-      <c r="T27">
-        <v>1</v>
-      </c>
-      <c r="U27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S28">
-        <v>1</v>
-      </c>
-      <c r="T28">
-        <v>0</v>
-      </c>
-      <c r="U28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S29">
-        <v>1</v>
-      </c>
-      <c r="T29">
-        <v>0</v>
-      </c>
-      <c r="U29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S30">
-        <v>1</v>
-      </c>
-      <c r="T30">
-        <v>1</v>
-      </c>
-      <c r="U30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S31">
-        <v>1</v>
-      </c>
-      <c r="T31">
-        <v>1</v>
-      </c>
-      <c r="U31">
-        <v>1</v>
-      </c>
+      <c r="E17" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A19:E19"/>
-    <mergeCell ref="W18:AB18"/>
-    <mergeCell ref="W11:AB11"/>
+    <mergeCell ref="M9:R9"/>
+    <mergeCell ref="M2:R2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82BA34EB-1C32-48FE-B512-5C5A618EAC32}">
   <dimension ref="A1:P5"/>
   <sheetViews>
@@ -3976,13 +4652,13 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="C1" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="M1">
         <v>0</v>
@@ -3999,10 +4675,10 @@
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C2" t="str">
         <f>DEC2BIN(1, 4)</f>
@@ -4011,10 +4687,10 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C3" t="str">
         <f>DEC2BIN(2, 4)</f>
@@ -4023,10 +4699,10 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C4" t="str">
         <f>DEC2BIN(4, 4)</f>
@@ -4035,10 +4711,10 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="C5" t="str">
         <f>DEC2BIN(8, 4)</f>
@@ -4050,12 +4726,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B656CCEA-8C5E-4FD9-9F21-21B7A6DC026C}">
   <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:P18"/>
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4087,15 +4763,15 @@
       <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
+      <c r="J1" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4177,15 +4853,15 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J8" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
+      <c r="J8" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
@@ -4197,15 +4873,15 @@
       <c r="L9" t="s">
         <v>50</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N9" s="4"/>
+      <c r="N9" s="5"/>
       <c r="P9" t="s">
         <v>57</v>
       </c>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
@@ -4217,10 +4893,10 @@
       <c r="L10">
         <v>2</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="5">
         <v>8</v>
       </c>
-      <c r="N10" s="4"/>
+      <c r="N10" s="5"/>
       <c r="P10">
         <f>SUM(K10:N10)</f>
         <v>16</v>
@@ -4235,73 +4911,82 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J15" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
+      <c r="J15" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J16" t="s">
+      <c r="J16" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="M16" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="N16" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="N16" s="4"/>
-      <c r="P16" t="s">
+      <c r="O16" s="6"/>
+      <c r="P16" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
     </row>
     <row r="17" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J17" t="s">
+      <c r="J17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="6">
         <v>6</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="6">
         <v>2</v>
       </c>
-      <c r="M17" s="4">
-        <v>8</v>
-      </c>
-      <c r="N17" s="4"/>
-      <c r="P17">
+      <c r="M17" s="39">
+        <v>4</v>
+      </c>
+      <c r="N17" s="39">
+        <v>4</v>
+      </c>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6">
         <f>SUM(K17:N17)</f>
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J18" t="s">
+      <c r="J18" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="L18" t="s">
+      <c r="K18" s="6"/>
+      <c r="L18" s="6" t="s">
         <v>56</v>
       </c>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
     </row>
     <row r="27" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="K27" s="20"/>
+      <c r="K27" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="5">
     <mergeCell ref="J8:P8"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="J15:P15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="M10:N10"/>
   </mergeCells>

</xml_diff>

<commit_message>
Interrupts - microcode + tests
</commit_message>
<xml_diff>
--- a/KPC8/Docs/Specs.xlsx
+++ b/KPC8/Docs/Specs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\kpc8\KPC8\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Random\KPC8\KPC8\KPC8\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DB2471-DF92-40F5-B01E-8F2E6250EB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7367B2B-3AD3-4192-9E33-49BEAF99EDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{17029D09-6E3C-4208-87C0-FA3EA582112B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{17029D09-6E3C-4208-87C0-FA3EA582112B}"/>
   </bookViews>
   <sheets>
     <sheet name="Control signals" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="393">
   <si>
     <t>OPCODE HEX</t>
   </si>
@@ -588,9 +588,6 @@
     <t>irrex</t>
   </si>
   <si>
-    <t>$zero, IMM</t>
-  </si>
-  <si>
     <t>lbext</t>
   </si>
   <si>
@@ -1179,16 +1176,49 @@
     <t>if (of) pc = $rAddress</t>
   </si>
   <si>
-    <t>IRR_ACK; pc = $rAddress</t>
-  </si>
-  <si>
     <t>$t1, #addressLo</t>
   </si>
   <si>
-    <t>IRR_ACK; $t1=pc; pc = FF|#addressLo</t>
-  </si>
-  <si>
-    <t>Interrupts may only use $t1-$t4 registers</t>
+    <t>Saved registers</t>
+  </si>
+  <si>
+    <t>PC_lo</t>
+  </si>
+  <si>
+    <t>FF00</t>
+  </si>
+  <si>
+    <t>PC_hi</t>
+  </si>
+  <si>
+    <t>FF01</t>
+  </si>
+  <si>
+    <t>Interrupts may only use $t1 by default. All other registers must be saved by interrupts</t>
+  </si>
+  <si>
+    <t>IRR_ACK; *(FF00)=pc; *(FF02)=$t1; pc = FF|#addressLo</t>
+  </si>
+  <si>
+    <t>$t1_hi</t>
+  </si>
+  <si>
+    <t>FF02</t>
+  </si>
+  <si>
+    <t>$t2_lo</t>
+  </si>
+  <si>
+    <t>FF03</t>
+  </si>
+  <si>
+    <t>Caution when using, as those addresses are used to store data between interrupts in RAM</t>
+  </si>
+  <si>
+    <t>$t1, #notused</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pc = *(FF00); $t1=*(FF02); IRR_ACK; </t>
   </si>
 </sst>
 </file>
@@ -1474,7 +1504,7 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1519,6 +1549,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -1561,20 +1594,24 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="20% — akcent 1" xfId="5" builtinId="30"/>
-    <cellStyle name="20% — akcent 2" xfId="6" builtinId="34"/>
-    <cellStyle name="40% — akcent 2" xfId="7" builtinId="35"/>
-    <cellStyle name="60% — akcent 3" xfId="8" builtinId="40"/>
-    <cellStyle name="Dane wejściowe" xfId="4" builtinId="20"/>
-    <cellStyle name="Dobry" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutralny" xfId="3" builtinId="28"/>
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
-    <cellStyle name="Zły" xfId="2" builtinId="27"/>
+    <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
+    <cellStyle name="20% - Accent2" xfId="6" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="7" builtinId="35"/>
+    <cellStyle name="60% - Accent3" xfId="8" builtinId="40"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="4" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1607,9 +1644,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1647,7 +1684,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1753,7 +1790,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1943,7 +1980,7 @@
         <f>ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="27" t="s">
         <v>94</v>
       </c>
       <c r="D2" t="s">
@@ -1958,7 +1995,7 @@
         <f t="shared" ref="A3:A32" si="0">ROW()-1</f>
         <v>2</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="28"/>
       <c r="D3" t="s">
         <v>65</v>
       </c>
@@ -1971,7 +2008,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C4" s="27"/>
+      <c r="C4" s="28"/>
       <c r="D4" t="s">
         <v>65</v>
       </c>
@@ -1984,7 +2021,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="C5" s="28"/>
       <c r="D5" t="s">
         <v>65</v>
       </c>
@@ -1997,7 +2034,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C6" s="27"/>
+      <c r="C6" s="28"/>
       <c r="D6" t="s">
         <v>66</v>
       </c>
@@ -2010,7 +2047,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="28"/>
       <c r="D7" t="s">
         <v>66</v>
       </c>
@@ -2023,7 +2060,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C8" s="27"/>
+      <c r="C8" s="28"/>
       <c r="D8" t="s">
         <v>66</v>
       </c>
@@ -2039,7 +2076,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C9" s="27"/>
+      <c r="C9" s="28"/>
       <c r="D9" t="s">
         <v>79</v>
       </c>
@@ -2052,7 +2089,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C10" s="27"/>
+      <c r="C10" s="28"/>
       <c r="D10" t="s">
         <v>66</v>
       </c>
@@ -2065,7 +2102,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="28"/>
       <c r="D11" t="s">
         <v>46</v>
       </c>
@@ -2078,7 +2115,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C12" s="27"/>
+      <c r="C12" s="28"/>
       <c r="D12" t="s">
         <v>46</v>
       </c>
@@ -2091,7 +2128,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C13" s="27"/>
+      <c r="C13" s="28"/>
       <c r="D13" t="s">
         <v>47</v>
       </c>
@@ -2104,7 +2141,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="29" t="s">
         <v>95</v>
       </c>
       <c r="D14" t="s">
@@ -2119,7 +2156,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C15" s="28"/>
+      <c r="C15" s="29"/>
       <c r="D15" t="s">
         <v>75</v>
       </c>
@@ -2132,7 +2169,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C16" s="28"/>
+      <c r="C16" s="29"/>
       <c r="D16" t="s">
         <v>75</v>
       </c>
@@ -2148,7 +2185,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C17" s="28"/>
+      <c r="C17" s="29"/>
       <c r="D17" t="s">
         <v>80</v>
       </c>
@@ -2161,7 +2198,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C18" s="28"/>
+      <c r="C18" s="29"/>
       <c r="D18" t="s">
         <v>81</v>
       </c>
@@ -2177,7 +2214,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C19" s="28"/>
+      <c r="C19" s="29"/>
       <c r="D19" t="s">
         <v>81</v>
       </c>
@@ -2190,7 +2227,7 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C20" s="28"/>
+      <c r="C20" s="29"/>
       <c r="D20" t="s">
         <v>96</v>
       </c>
@@ -2203,7 +2240,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C21" s="28"/>
+      <c r="C21" s="29"/>
       <c r="D21" t="s">
         <v>97</v>
       </c>
@@ -2216,7 +2253,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C22" s="28"/>
+      <c r="C22" s="29"/>
       <c r="D22" t="s">
         <v>98</v>
       </c>
@@ -2229,7 +2266,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="31" t="s">
         <v>82</v>
       </c>
       <c r="D23" t="s">
@@ -2244,7 +2281,7 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C24" s="30"/>
+      <c r="C24" s="31"/>
       <c r="D24" t="s">
         <v>82</v>
       </c>
@@ -2257,7 +2294,7 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="30" t="s">
         <v>83</v>
       </c>
       <c r="D25" t="s">
@@ -2272,7 +2309,7 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C26" s="29"/>
+      <c r="C26" s="30"/>
       <c r="D26" t="s">
         <v>73</v>
       </c>
@@ -2288,7 +2325,7 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C27" s="29"/>
+      <c r="C27" s="30"/>
       <c r="D27" t="s">
         <v>76</v>
       </c>
@@ -2301,7 +2338,7 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="C28" s="29"/>
+      <c r="C28" s="30"/>
       <c r="D28" t="s">
         <v>74</v>
       </c>
@@ -2314,7 +2351,7 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C29" s="29"/>
+      <c r="C29" s="30"/>
       <c r="D29" t="s">
         <v>74</v>
       </c>
@@ -2330,7 +2367,7 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="C30" s="29"/>
+      <c r="C30" s="30"/>
       <c r="D30" t="s">
         <v>78</v>
       </c>
@@ -2343,7 +2380,7 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="C31" s="29"/>
+      <c r="C31" s="30"/>
       <c r="D31" t="s">
         <v>83</v>
       </c>
@@ -2356,7 +2393,7 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="C32" s="29"/>
+      <c r="C32" s="30"/>
       <c r="D32" t="s">
         <v>83</v>
       </c>
@@ -2437,20 +2474,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F904DBB9-1FEB-4077-A5E6-86A97D866F70}">
   <dimension ref="A1:W70"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54:I57"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.85546875" style="4" customWidth="1"/>
     <col min="6" max="6" width="38.7109375" style="4" customWidth="1"/>
     <col min="7" max="7" width="53" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35" customWidth="1"/>
+    <col min="8" max="8" width="48.42578125" customWidth="1"/>
     <col min="9" max="9" width="31.5703125" customWidth="1"/>
     <col min="19" max="19" width="17.140625" customWidth="1"/>
     <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
@@ -2476,13 +2512,13 @@
         <v>174</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>54</v>
@@ -2496,7 +2532,7 @@
         <f>DEC2HEX(_xlfn.NUMBERVALUE( ROW()-2),2)</f>
         <v>00</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>108</v>
       </c>
       <c r="C2" t="str">
@@ -2507,7 +2543,7 @@
         <v>60</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>61</v>
@@ -2521,7 +2557,7 @@
         <f t="shared" ref="A3:A65" si="0">DEC2HEX(_xlfn.NUMBERVALUE( ROW()-2),2)</f>
         <v>01</v>
       </c>
-      <c r="B3" s="35"/>
+      <c r="B3" s="36"/>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C65" si="1">HEX2BIN(A3,6)</f>
         <v>000001</v>
@@ -2530,16 +2566,16 @@
         <v>165</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>168</v>
       </c>
       <c r="H3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="W3" t="s">
         <v>42</v>
@@ -2550,25 +2586,25 @@
         <f t="shared" si="0"/>
         <v>02</v>
       </c>
-      <c r="B4" s="35"/>
+      <c r="B4" s="36"/>
       <c r="C4" t="str">
         <f t="shared" si="1"/>
         <v>000010</v>
       </c>
       <c r="D4" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>204</v>
-      </c>
       <c r="H4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I4" s="4"/>
       <c r="W4" t="s">
@@ -2580,7 +2616,7 @@
         <f t="shared" si="0"/>
         <v>03</v>
       </c>
-      <c r="B5" s="35"/>
+      <c r="B5" s="36"/>
       <c r="C5" t="str">
         <f t="shared" si="1"/>
         <v>000011</v>
@@ -2589,16 +2625,16 @@
         <v>166</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>169</v>
       </c>
       <c r="H5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -2606,25 +2642,25 @@
         <f t="shared" si="0"/>
         <v>04</v>
       </c>
-      <c r="B6" s="35"/>
+      <c r="B6" s="36"/>
       <c r="C6" t="str">
         <f t="shared" si="1"/>
         <v>000100</v>
       </c>
       <c r="D6" s="22" t="s">
+        <v>309</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" t="s">
         <v>312</v>
-      </c>
-      <c r="H6" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -2632,7 +2668,7 @@
         <f t="shared" si="0"/>
         <v>05</v>
       </c>
-      <c r="B7" s="35"/>
+      <c r="B7" s="36"/>
       <c r="C7" t="str">
         <f t="shared" si="1"/>
         <v>000101</v>
@@ -2641,16 +2677,16 @@
         <v>170</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>62</v>
       </c>
       <c r="H7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -2658,25 +2694,25 @@
         <f t="shared" si="0"/>
         <v>06</v>
       </c>
-      <c r="B8" s="35"/>
+      <c r="B8" s="36"/>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
         <v>000110</v>
       </c>
       <c r="D8" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>223</v>
-      </c>
       <c r="H8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -2684,7 +2720,7 @@
         <f t="shared" si="0"/>
         <v>07</v>
       </c>
-      <c r="B9" s="35"/>
+      <c r="B9" s="36"/>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
         <v>000111</v>
@@ -2693,16 +2729,16 @@
         <v>171</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>167</v>
       </c>
       <c r="H9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -2710,25 +2746,25 @@
         <f t="shared" si="0"/>
         <v>08</v>
       </c>
-      <c r="B10" s="35"/>
+      <c r="B10" s="36"/>
       <c r="C10" t="str">
         <f t="shared" si="1"/>
         <v>001000</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>315</v>
-      </c>
       <c r="H10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -2736,25 +2772,25 @@
         <f t="shared" si="0"/>
         <v>09</v>
       </c>
-      <c r="B11" s="35"/>
+      <c r="B11" s="36"/>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
         <v>001001</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -2762,25 +2798,25 @@
         <f t="shared" si="0"/>
         <v>0A</v>
       </c>
-      <c r="B12" s="35"/>
+      <c r="B12" s="36"/>
       <c r="C12" t="str">
         <f t="shared" si="1"/>
         <v>001010</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -2788,19 +2824,19 @@
         <f t="shared" si="0"/>
         <v>0B</v>
       </c>
-      <c r="B13" s="35"/>
+      <c r="B13" s="36"/>
       <c r="C13" t="str">
         <f t="shared" si="1"/>
         <v>001011</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -2808,7 +2844,7 @@
         <f t="shared" si="0"/>
         <v>0C</v>
       </c>
-      <c r="B14" s="35"/>
+      <c r="B14" s="36"/>
       <c r="C14" t="str">
         <f t="shared" si="1"/>
         <v>001100</v>
@@ -2817,10 +2853,10 @@
         <v>172</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -2828,19 +2864,19 @@
         <f t="shared" si="0"/>
         <v>0D</v>
       </c>
-      <c r="B15" s="35"/>
+      <c r="B15" s="36"/>
       <c r="C15" t="str">
         <f t="shared" si="1"/>
         <v>001101</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -2848,19 +2884,19 @@
         <f t="shared" si="0"/>
         <v>0E</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="36"/>
       <c r="C16" t="str">
         <f t="shared" si="1"/>
         <v>001110</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2868,7 +2904,7 @@
         <f t="shared" si="0"/>
         <v>0F</v>
       </c>
-      <c r="B17" s="35"/>
+      <c r="B17" s="36"/>
       <c r="C17" t="str">
         <f t="shared" si="1"/>
         <v>001111</v>
@@ -2877,10 +2913,10 @@
         <v>173</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2888,19 +2924,19 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B18" s="35"/>
+      <c r="B18" s="36"/>
       <c r="C18" t="str">
         <f t="shared" si="1"/>
         <v>010000</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2908,25 +2944,25 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="36"/>
       <c r="C19" t="str">
         <f t="shared" si="1"/>
         <v>010001</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2934,25 +2970,25 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B20" s="35"/>
+      <c r="B20" s="36"/>
       <c r="C20" t="str">
         <f t="shared" si="1"/>
         <v>010010</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G20" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2960,19 +2996,19 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B21" s="35"/>
+      <c r="B21" s="36"/>
       <c r="C21" t="str">
         <f t="shared" si="1"/>
         <v>010011</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2980,7 +3016,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B22" s="35"/>
+      <c r="B22" s="36"/>
       <c r="C22" t="str">
         <f t="shared" si="1"/>
         <v>010100</v>
@@ -2992,10 +3028,10 @@
         <v>177</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -3003,7 +3039,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B23" s="35"/>
+      <c r="B23" s="36"/>
       <c r="C23" t="str">
         <f t="shared" si="1"/>
         <v>010101</v>
@@ -3012,13 +3048,13 @@
         <v>178</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3026,7 +3062,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B24" s="35"/>
+      <c r="B24" s="36"/>
       <c r="C24" t="str">
         <f t="shared" si="1"/>
         <v>010110</v>
@@ -3038,13 +3074,13 @@
         <v>177</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H24" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -3052,7 +3088,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="36"/>
       <c r="C25" t="str">
         <f t="shared" si="1"/>
         <v>010111</v>
@@ -3061,16 +3097,16 @@
         <v>180</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -3078,25 +3114,25 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B26" s="35"/>
+      <c r="B26" s="36"/>
       <c r="C26" t="str">
         <f t="shared" si="1"/>
         <v>011000</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>177</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -3104,25 +3140,25 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B27" s="35"/>
+      <c r="B27" s="36"/>
       <c r="C27" t="str">
         <f t="shared" si="1"/>
         <v>011001</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -3130,22 +3166,22 @@
         <f t="shared" si="0"/>
         <v>1A</v>
       </c>
-      <c r="B28" s="35"/>
+      <c r="B28" s="36"/>
       <c r="C28" t="str">
         <f t="shared" si="1"/>
         <v>011010</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>177</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H28" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3153,22 +3189,22 @@
         <f t="shared" si="0"/>
         <v>1B</v>
       </c>
-      <c r="B29" s="35"/>
+      <c r="B29" s="36"/>
       <c r="C29" t="str">
         <f t="shared" si="1"/>
         <v>011011</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>177</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3176,22 +3212,22 @@
         <f t="shared" si="0"/>
         <v>1C</v>
       </c>
-      <c r="B30" s="35"/>
+      <c r="B30" s="36"/>
       <c r="C30" t="str">
         <f t="shared" si="1"/>
         <v>011100</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>177</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -3199,22 +3235,22 @@
         <f t="shared" si="0"/>
         <v>1D</v>
       </c>
-      <c r="B31" s="35"/>
+      <c r="B31" s="36"/>
       <c r="C31" t="str">
         <f t="shared" si="1"/>
         <v>011101</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>177</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H31" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3222,22 +3258,22 @@
         <f t="shared" si="0"/>
         <v>1E</v>
       </c>
-      <c r="B32" s="35"/>
+      <c r="B32" s="36"/>
       <c r="C32" t="str">
         <f t="shared" si="1"/>
         <v>011110</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>177</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H32" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3245,22 +3281,22 @@
         <f t="shared" si="0"/>
         <v>1F</v>
       </c>
-      <c r="B33" s="35"/>
+      <c r="B33" s="36"/>
       <c r="C33" t="str">
         <f t="shared" si="1"/>
         <v>011111</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>177</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H33" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3268,25 +3304,25 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B34" s="35"/>
+      <c r="B34" s="36"/>
       <c r="C34" t="str">
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G34" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3294,25 +3330,25 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B35" s="35"/>
+      <c r="B35" s="36"/>
       <c r="C35" t="str">
         <f t="shared" si="1"/>
         <v>100001</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G35" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H35" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3320,25 +3356,25 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B36" s="35"/>
+      <c r="B36" s="36"/>
       <c r="C36" t="str">
         <f t="shared" si="1"/>
         <v>100010</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G36" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H36" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -3346,25 +3382,25 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B37" s="35"/>
+      <c r="B37" s="36"/>
       <c r="C37" t="str">
         <f t="shared" si="1"/>
         <v>100011</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F37" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="G37" t="s">
         <v>265</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>266</v>
-      </c>
-      <c r="H37" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -3372,22 +3408,22 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B38" s="35"/>
+      <c r="B38" s="36"/>
       <c r="C38" t="str">
         <f t="shared" si="1"/>
         <v>100100</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E38" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="H38" t="s">
         <v>216</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="H38" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3395,22 +3431,22 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B39" s="35"/>
+      <c r="B39" s="36"/>
       <c r="C39" t="str">
         <f t="shared" si="1"/>
         <v>100101</v>
       </c>
       <c r="D39" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="H39" t="s">
         <v>279</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="H39" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3418,22 +3454,22 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B40" s="35"/>
+      <c r="B40" s="36"/>
       <c r="C40" t="str">
         <f t="shared" si="1"/>
         <v>100110</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H40" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -3441,22 +3477,22 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B41" s="35"/>
+      <c r="B41" s="36"/>
       <c r="C41" t="str">
         <f t="shared" si="1"/>
         <v>100111</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H41" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3464,22 +3500,22 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B42" s="35"/>
+      <c r="B42" s="36"/>
       <c r="C42" t="str">
         <f t="shared" si="1"/>
         <v>101000</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H42" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3487,22 +3523,22 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B43" s="35"/>
+      <c r="B43" s="36"/>
       <c r="C43" t="str">
         <f t="shared" si="1"/>
         <v>101001</v>
       </c>
       <c r="D43" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="H43" t="s">
         <v>275</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="H43" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3510,22 +3546,22 @@
         <f t="shared" si="0"/>
         <v>2A</v>
       </c>
-      <c r="B44" s="35"/>
+      <c r="B44" s="36"/>
       <c r="C44" t="str">
         <f t="shared" si="1"/>
         <v>101010</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H44" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3533,25 +3569,25 @@
         <f t="shared" si="0"/>
         <v>2B</v>
       </c>
-      <c r="B45" s="35"/>
+      <c r="B45" s="36"/>
       <c r="C45" t="str">
         <f t="shared" si="1"/>
         <v>101011</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E45" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="G45" t="s">
         <v>192</v>
       </c>
-      <c r="F45" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="G45" t="s">
-        <v>193</v>
-      </c>
       <c r="H45" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -3559,25 +3595,25 @@
         <f t="shared" si="0"/>
         <v>2C</v>
       </c>
-      <c r="B46" s="35"/>
+      <c r="B46" s="36"/>
       <c r="C46" t="str">
         <f t="shared" si="1"/>
         <v>101100</v>
       </c>
       <c r="D46" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="F46" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="G46" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="F46" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="G46" s="4" t="s">
+      <c r="H46" s="4" t="s">
         <v>340</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3585,28 +3621,28 @@
         <f t="shared" si="0"/>
         <v>2D</v>
       </c>
-      <c r="B47" s="35"/>
+      <c r="B47" s="36"/>
       <c r="C47" t="str">
         <f t="shared" si="1"/>
         <v>101101</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E47" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="G47" t="s">
         <v>197</v>
       </c>
-      <c r="F47" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="G47" t="s">
-        <v>198</v>
-      </c>
       <c r="H47" t="s">
+        <v>332</v>
+      </c>
+      <c r="I47" t="s">
         <v>333</v>
-      </c>
-      <c r="I47" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -3614,28 +3650,28 @@
         <f t="shared" si="0"/>
         <v>2E</v>
       </c>
-      <c r="B48" s="35"/>
+      <c r="B48" s="36"/>
       <c r="C48" t="str">
         <f t="shared" si="1"/>
         <v>101110</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G48" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H48" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I48" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3643,7 +3679,7 @@
         <f t="shared" si="0"/>
         <v>2F</v>
       </c>
-      <c r="B49" s="35"/>
+      <c r="B49" s="36"/>
       <c r="C49" t="str">
         <f t="shared" si="1"/>
         <v>101111</v>
@@ -3654,7 +3690,7 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B50" s="35"/>
+      <c r="B50" s="36"/>
       <c r="C50" t="str">
         <f t="shared" si="1"/>
         <v>110000</v>
@@ -3665,7 +3701,7 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B51" s="35"/>
+      <c r="B51" s="36"/>
       <c r="C51" t="str">
         <f t="shared" si="1"/>
         <v>110001</v>
@@ -3676,7 +3712,7 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B52" s="35"/>
+      <c r="B52" s="36"/>
       <c r="C52" t="str">
         <f t="shared" si="1"/>
         <v>110010</v>
@@ -3687,35 +3723,35 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B53" s="36"/>
+      <c r="B53" s="37"/>
       <c r="C53" t="str">
         <f t="shared" si="1"/>
         <v>110011</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="str">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B54" s="32" t="s">
+      <c r="B54" s="33" t="s">
         <v>145</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="1"/>
         <v>110100</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="22" t="s">
         <v>181</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="H54" s="40" t="s">
-        <v>381</v>
+      <c r="H54" s="26" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3723,22 +3759,22 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B55" s="33"/>
+      <c r="B55" s="34"/>
       <c r="C55" t="str">
         <f t="shared" si="1"/>
         <v>110101</v>
       </c>
-      <c r="D55" t="s">
-        <v>185</v>
+      <c r="D55" s="22" t="s">
+        <v>184</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>190</v>
+        <v>391</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="H55" s="40" t="s">
-        <v>379</v>
+      <c r="H55" s="26" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3746,16 +3782,16 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B56" s="33"/>
+      <c r="B56" s="34"/>
       <c r="C56" t="str">
         <f t="shared" si="1"/>
         <v>110110</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="22" t="s">
         <v>142</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>182</v>
+        <v>391</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>143</v>
@@ -3766,16 +3802,16 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B57" s="34"/>
+      <c r="B57" s="35"/>
       <c r="C57" t="str">
         <f t="shared" si="1"/>
         <v>110111</v>
       </c>
-      <c r="D57" t="s">
-        <v>186</v>
+      <c r="D57" s="22" t="s">
+        <v>185</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>182</v>
+        <v>391</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>144</v>
@@ -3786,7 +3822,7 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B58" s="31" t="s">
+      <c r="B58" s="32" t="s">
         <v>109</v>
       </c>
       <c r="C58" t="str">
@@ -3794,19 +3830,19 @@
         <v>111000</v>
       </c>
       <c r="D58" s="22" t="s">
+        <v>345</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="F58" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="E58" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>347</v>
-      </c>
       <c r="G58" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3814,25 +3850,25 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B59" s="31"/>
+      <c r="B59" s="32"/>
       <c r="C59" t="str">
         <f t="shared" si="1"/>
         <v>111001</v>
       </c>
       <c r="D59" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="F59" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="E59" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>361</v>
-      </c>
       <c r="G59" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3840,25 +3876,25 @@
         <f t="shared" si="0"/>
         <v>3A</v>
       </c>
-      <c r="B60" s="31"/>
+      <c r="B60" s="32"/>
       <c r="C60" t="str">
         <f t="shared" si="1"/>
         <v>111010</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3866,25 +3902,25 @@
         <f t="shared" si="0"/>
         <v>3B</v>
       </c>
-      <c r="B61" s="31"/>
+      <c r="B61" s="32"/>
       <c r="C61" t="str">
         <f t="shared" si="1"/>
         <v>111011</v>
       </c>
       <c r="D61" s="22" t="s">
+        <v>365</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="G61" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="E61" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="F61" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="G61" s="4" t="s">
+      <c r="H61" s="4" t="s">
         <v>367</v>
-      </c>
-      <c r="H61" s="4" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3892,28 +3928,28 @@
         <f t="shared" si="0"/>
         <v>3C</v>
       </c>
-      <c r="B62" s="31"/>
+      <c r="B62" s="32"/>
       <c r="C62" t="str">
         <f t="shared" si="1"/>
         <v>111100</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3921,28 +3957,28 @@
         <f t="shared" si="0"/>
         <v>3D</v>
       </c>
-      <c r="B63" s="31"/>
+      <c r="B63" s="32"/>
       <c r="C63" t="str">
         <f t="shared" si="1"/>
         <v>111101</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3950,28 +3986,28 @@
         <f t="shared" si="0"/>
         <v>3E</v>
       </c>
-      <c r="B64" s="31"/>
+      <c r="B64" s="32"/>
       <c r="C64" t="str">
         <f t="shared" si="1"/>
         <v>111110</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3979,28 +4015,28 @@
         <f t="shared" si="0"/>
         <v>3F</v>
       </c>
-      <c r="B65" s="31"/>
+      <c r="B65" s="32"/>
       <c r="C65" t="str">
         <f t="shared" si="1"/>
         <v>111111</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -4060,10 +4096,10 @@
         <v>115</v>
       </c>
       <c r="D1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1" t="s">
         <v>240</v>
-      </c>
-      <c r="E1" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4077,7 +4113,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>92</v>
@@ -4097,7 +4133,7 @@
         <v>92</v>
       </c>
       <c r="E3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -4111,10 +4147,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -4131,7 +4167,7 @@
         <v>92</v>
       </c>
       <c r="E5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -4148,7 +4184,7 @@
         <v>92</v>
       </c>
       <c r="E6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -4165,7 +4201,7 @@
         <v>92</v>
       </c>
       <c r="E7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -4179,10 +4215,10 @@
         <v>0</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -4196,15 +4232,15 @@
         <v>1</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D10" s="24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -4214,10 +4250,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6777839-035A-4695-B7B0-93449B7EEA83}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:E23"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4225,6 +4261,7 @@
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
     <col min="10" max="10" width="19.140625" customWidth="1"/>
     <col min="11" max="11" width="19.5703125" customWidth="1"/>
     <col min="12" max="12" width="24.85546875" bestFit="1" customWidth="1"/>
@@ -4248,15 +4285,18 @@
       <c r="E1" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="F1" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
@@ -4662,32 +4702,35 @@
         <f t="shared" si="3"/>
         <v>00010000</v>
       </c>
-      <c r="J16" s="37" t="s">
+      <c r="J16" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
+      <c r="A17" s="5" t="str">
         <f t="shared" si="0"/>
         <v>0F</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B17" s="5" t="str">
         <f t="shared" si="1"/>
         <v>1111</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" s="5" t="str">
         <f t="shared" si="2"/>
         <v>FF00</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="5">
         <v>11010000</v>
       </c>
-      <c r="E17" t="str">
+      <c r="E17" s="5" t="str">
         <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
+      <c r="F17" s="42" t="s">
+        <v>390</v>
+      </c>
       <c r="J17" t="s">
         <v>149</v>
       </c>
@@ -4699,6 +4742,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F18" s="42"/>
       <c r="J18">
         <v>0</v>
       </c>
@@ -4710,6 +4754,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F19" s="42"/>
       <c r="J19">
         <v>0</v>
       </c>
@@ -4721,6 +4766,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F20" s="42"/>
       <c r="J20">
         <v>1</v>
       </c>
@@ -4735,12 +4781,12 @@
       <c r="A21" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="38" t="s">
-        <v>382</v>
-      </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
+      <c r="B21" s="43" t="s">
+        <v>384</v>
+      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
       <c r="J21">
         <v>1</v>
       </c>
@@ -4752,22 +4798,60 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>382</v>
+      </c>
+      <c r="B27" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>380</v>
+      </c>
+      <c r="B28" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>386</v>
+      </c>
+      <c r="B29" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>388</v>
+      </c>
+      <c r="B30" t="s">
+        <v>389</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="I1:O1"/>
     <mergeCell ref="J16:L16"/>
     <mergeCell ref="B21:E23"/>
+    <mergeCell ref="F17:F20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4779,7 +4863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6D5924-FD18-48E3-8129-A5F6A2CED0D8}">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
@@ -4858,14 +4942,14 @@
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="M2" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
@@ -4911,7 +4995,7 @@
         <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -4942,7 +5026,7 @@
         <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -5093,14 +5177,14 @@
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="M9" s="38" t="s">
+      <c r="M9" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="N9" s="38"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="38"/>
-      <c r="R9" s="38"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="39"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
@@ -5230,15 +5314,15 @@
         <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5379,15 +5463,15 @@
       <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -5469,15 +5553,15 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J8" s="38" t="s">
+      <c r="J8" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
@@ -5489,10 +5573,10 @@
       <c r="L9" t="s">
         <v>50</v>
       </c>
-      <c r="M9" s="38" t="s">
+      <c r="M9" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="N9" s="38"/>
+      <c r="N9" s="39"/>
       <c r="P9" t="s">
         <v>57</v>
       </c>
@@ -5509,10 +5593,10 @@
       <c r="L10">
         <v>2</v>
       </c>
-      <c r="M10" s="38">
+      <c r="M10" s="39">
         <v>8</v>
       </c>
-      <c r="N10" s="38"/>
+      <c r="N10" s="39"/>
       <c r="P10">
         <f>SUM(K10:N10)</f>
         <v>16</v>
@@ -5527,15 +5611,15 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J15" s="39" t="s">
-        <v>199</v>
-      </c>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
+      <c r="J15" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J16" s="5" t="s">

</xml_diff>

<commit_message>
Fibonacci and multiplication program tests + fixes
</commit_message>
<xml_diff>
--- a/KPC8/Docs/Specs.xlsx
+++ b/KPC8/Docs/Specs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Random\KPC8\KPC8\KPC8\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7367B2B-3AD3-4192-9E33-49BEAF99EDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94571D4-24CA-4379-91C4-D8A71E134D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{17029D09-6E3C-4208-87C0-FA3EA582112B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{17029D09-6E3C-4208-87C0-FA3EA582112B}"/>
   </bookViews>
   <sheets>
     <sheet name="Control signals" sheetId="4" r:id="rId1"/>
@@ -741,9 +741,6 @@
     <t>*$rAddress = $rA; $rAddress += 2</t>
   </si>
   <si>
-    <t>$rA = *$rAddress; $rAddress -= 2</t>
-  </si>
-  <si>
     <t>subtract</t>
   </si>
   <si>
@@ -816,12 +813,6 @@
     <t>negw</t>
   </si>
   <si>
-    <t>load byte from RAM and decrement $rAddress by 1</t>
-  </si>
-  <si>
-    <t>load word from RAM and decrement $rAddress by 2</t>
-  </si>
-  <si>
     <t>store byte in RAM and increment $rAddress by 1</t>
   </si>
   <si>
@@ -921,9 +912,6 @@
     <t>$rDest_lo = ($rA_lo + $rB_lo) &gt;&gt; 1</t>
   </si>
   <si>
-    <t>$rA_lo = *$rAddress; $rAddress -= 1</t>
-  </si>
-  <si>
     <t>*$rAddress = $rA_lo; $rAddress += 1</t>
   </si>
   <si>
@@ -1219,6 +1207,18 @@
   </si>
   <si>
     <t xml:space="preserve">pc = *(FF00); $t1=*(FF02); IRR_ACK; </t>
+  </si>
+  <si>
+    <t>decrement $rAddress by 2 and load word from RAM</t>
+  </si>
+  <si>
+    <t>decrement $rAddress by 1 and load byte from RAM</t>
+  </si>
+  <si>
+    <t>$rAddress -= 2; $rA = *$rAddress;</t>
+  </si>
+  <si>
+    <t>$rAddress -= 1; $rA_lo = *$rAddress;</t>
   </si>
 </sst>
 </file>
@@ -1552,6 +1552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -1589,17 +1590,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1980,7 +1980,7 @@
         <f>ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="28" t="s">
         <v>94</v>
       </c>
       <c r="D2" t="s">
@@ -1995,7 +1995,7 @@
         <f t="shared" ref="A3:A32" si="0">ROW()-1</f>
         <v>2</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="29"/>
       <c r="D3" t="s">
         <v>65</v>
       </c>
@@ -2008,7 +2008,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="29"/>
       <c r="D4" t="s">
         <v>65</v>
       </c>
@@ -2021,7 +2021,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="29"/>
       <c r="D5" t="s">
         <v>65</v>
       </c>
@@ -2034,7 +2034,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="29"/>
       <c r="D6" t="s">
         <v>66</v>
       </c>
@@ -2047,7 +2047,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="29"/>
       <c r="D7" t="s">
         <v>66</v>
       </c>
@@ -2060,7 +2060,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="29"/>
       <c r="D8" t="s">
         <v>66</v>
       </c>
@@ -2076,7 +2076,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C9" s="28"/>
+      <c r="C9" s="29"/>
       <c r="D9" t="s">
         <v>79</v>
       </c>
@@ -2089,7 +2089,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C10" s="28"/>
+      <c r="C10" s="29"/>
       <c r="D10" t="s">
         <v>66</v>
       </c>
@@ -2102,7 +2102,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="29"/>
       <c r="D11" t="s">
         <v>46</v>
       </c>
@@ -2115,7 +2115,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C12" s="28"/>
+      <c r="C12" s="29"/>
       <c r="D12" t="s">
         <v>46</v>
       </c>
@@ -2128,7 +2128,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C13" s="28"/>
+      <c r="C13" s="29"/>
       <c r="D13" t="s">
         <v>47</v>
       </c>
@@ -2141,7 +2141,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="30" t="s">
         <v>95</v>
       </c>
       <c r="D14" t="s">
@@ -2156,7 +2156,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C15" s="29"/>
+      <c r="C15" s="30"/>
       <c r="D15" t="s">
         <v>75</v>
       </c>
@@ -2169,7 +2169,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C16" s="29"/>
+      <c r="C16" s="30"/>
       <c r="D16" t="s">
         <v>75</v>
       </c>
@@ -2185,7 +2185,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C17" s="29"/>
+      <c r="C17" s="30"/>
       <c r="D17" t="s">
         <v>80</v>
       </c>
@@ -2198,7 +2198,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C18" s="29"/>
+      <c r="C18" s="30"/>
       <c r="D18" t="s">
         <v>81</v>
       </c>
@@ -2214,7 +2214,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C19" s="29"/>
+      <c r="C19" s="30"/>
       <c r="D19" t="s">
         <v>81</v>
       </c>
@@ -2227,7 +2227,7 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C20" s="29"/>
+      <c r="C20" s="30"/>
       <c r="D20" t="s">
         <v>96</v>
       </c>
@@ -2240,7 +2240,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C21" s="29"/>
+      <c r="C21" s="30"/>
       <c r="D21" t="s">
         <v>97</v>
       </c>
@@ -2253,7 +2253,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C22" s="29"/>
+      <c r="C22" s="30"/>
       <c r="D22" t="s">
         <v>98</v>
       </c>
@@ -2266,7 +2266,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="32" t="s">
         <v>82</v>
       </c>
       <c r="D23" t="s">
@@ -2281,7 +2281,7 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C24" s="31"/>
+      <c r="C24" s="32"/>
       <c r="D24" t="s">
         <v>82</v>
       </c>
@@ -2294,7 +2294,7 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="31" t="s">
         <v>83</v>
       </c>
       <c r="D25" t="s">
@@ -2309,7 +2309,7 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C26" s="30"/>
+      <c r="C26" s="31"/>
       <c r="D26" t="s">
         <v>73</v>
       </c>
@@ -2325,7 +2325,7 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C27" s="30"/>
+      <c r="C27" s="31"/>
       <c r="D27" t="s">
         <v>76</v>
       </c>
@@ -2338,7 +2338,7 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="C28" s="30"/>
+      <c r="C28" s="31"/>
       <c r="D28" t="s">
         <v>74</v>
       </c>
@@ -2351,7 +2351,7 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C29" s="30"/>
+      <c r="C29" s="31"/>
       <c r="D29" t="s">
         <v>74</v>
       </c>
@@ -2367,7 +2367,7 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="C30" s="30"/>
+      <c r="C30" s="31"/>
       <c r="D30" t="s">
         <v>78</v>
       </c>
@@ -2380,7 +2380,7 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="C31" s="30"/>
+      <c r="C31" s="31"/>
       <c r="D31" t="s">
         <v>83</v>
       </c>
@@ -2393,7 +2393,7 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="C32" s="30"/>
+      <c r="C32" s="31"/>
       <c r="D32" t="s">
         <v>83</v>
       </c>
@@ -2474,8 +2474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F904DBB9-1FEB-4077-A5E6-86A97D866F70}">
   <dimension ref="A1:W70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2532,7 +2532,7 @@
         <f>DEC2HEX(_xlfn.NUMBERVALUE( ROW()-2),2)</f>
         <v>00</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>108</v>
       </c>
       <c r="C2" t="str">
@@ -2557,7 +2557,7 @@
         <f t="shared" ref="A3:A65" si="0">DEC2HEX(_xlfn.NUMBERVALUE( ROW()-2),2)</f>
         <v>01</v>
       </c>
-      <c r="B3" s="36"/>
+      <c r="B3" s="37"/>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C65" si="1">HEX2BIN(A3,6)</f>
         <v>000001</v>
@@ -2575,7 +2575,7 @@
         <v>168</v>
       </c>
       <c r="H3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="W3" t="s">
         <v>42</v>
@@ -2586,7 +2586,7 @@
         <f t="shared" si="0"/>
         <v>02</v>
       </c>
-      <c r="B4" s="36"/>
+      <c r="B4" s="37"/>
       <c r="C4" t="str">
         <f t="shared" si="1"/>
         <v>000010</v>
@@ -2604,7 +2604,7 @@
         <v>203</v>
       </c>
       <c r="H4" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="I4" s="4"/>
       <c r="W4" t="s">
@@ -2616,7 +2616,7 @@
         <f t="shared" si="0"/>
         <v>03</v>
       </c>
-      <c r="B5" s="36"/>
+      <c r="B5" s="37"/>
       <c r="C5" t="str">
         <f t="shared" si="1"/>
         <v>000011</v>
@@ -2642,25 +2642,25 @@
         <f t="shared" si="0"/>
         <v>04</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="37"/>
       <c r="C6" t="str">
         <f t="shared" si="1"/>
         <v>000100</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>193</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="H6" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -2668,7 +2668,7 @@
         <f t="shared" si="0"/>
         <v>05</v>
       </c>
-      <c r="B7" s="36"/>
+      <c r="B7" s="37"/>
       <c r="C7" t="str">
         <f t="shared" si="1"/>
         <v>000101</v>
@@ -2686,7 +2686,7 @@
         <v>62</v>
       </c>
       <c r="H7" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -2694,7 +2694,7 @@
         <f t="shared" si="0"/>
         <v>06</v>
       </c>
-      <c r="B8" s="36"/>
+      <c r="B8" s="37"/>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
         <v>000110</v>
@@ -2712,7 +2712,7 @@
         <v>222</v>
       </c>
       <c r="H8" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -2720,7 +2720,7 @@
         <f t="shared" si="0"/>
         <v>07</v>
       </c>
-      <c r="B9" s="36"/>
+      <c r="B9" s="37"/>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
         <v>000111</v>
@@ -2746,25 +2746,25 @@
         <f t="shared" si="0"/>
         <v>08</v>
       </c>
-      <c r="B10" s="36"/>
+      <c r="B10" s="37"/>
       <c r="C10" t="str">
         <f t="shared" si="1"/>
         <v>001000</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>193</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H10" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -2772,7 +2772,7 @@
         <f t="shared" si="0"/>
         <v>09</v>
       </c>
-      <c r="B11" s="36"/>
+      <c r="B11" s="37"/>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
         <v>001001</v>
@@ -2787,10 +2787,10 @@
         <v>230</v>
       </c>
       <c r="G11" t="s">
-        <v>258</v>
+        <v>390</v>
       </c>
       <c r="H11" t="s">
-        <v>293</v>
+        <v>392</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -2798,7 +2798,7 @@
         <f t="shared" si="0"/>
         <v>0A</v>
       </c>
-      <c r="B12" s="36"/>
+      <c r="B12" s="37"/>
       <c r="C12" t="str">
         <f t="shared" si="1"/>
         <v>001010</v>
@@ -2813,10 +2813,10 @@
         <v>231</v>
       </c>
       <c r="G12" t="s">
-        <v>259</v>
+        <v>389</v>
       </c>
       <c r="H12" t="s">
-        <v>233</v>
+        <v>391</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -2824,7 +2824,7 @@
         <f t="shared" si="0"/>
         <v>0B</v>
       </c>
-      <c r="B13" s="36"/>
+      <c r="B13" s="37"/>
       <c r="C13" t="str">
         <f t="shared" si="1"/>
         <v>001011</v>
@@ -2836,7 +2836,7 @@
         <v>199</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -2844,7 +2844,7 @@
         <f t="shared" si="0"/>
         <v>0C</v>
       </c>
-      <c r="B14" s="36"/>
+      <c r="B14" s="37"/>
       <c r="C14" t="str">
         <f t="shared" si="1"/>
         <v>001100</v>
@@ -2853,10 +2853,10 @@
         <v>172</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -2864,7 +2864,7 @@
         <f t="shared" si="0"/>
         <v>0D</v>
       </c>
-      <c r="B15" s="36"/>
+      <c r="B15" s="37"/>
       <c r="C15" t="str">
         <f t="shared" si="1"/>
         <v>001101</v>
@@ -2873,10 +2873,10 @@
         <v>188</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -2884,19 +2884,19 @@
         <f t="shared" si="0"/>
         <v>0E</v>
       </c>
-      <c r="B16" s="36"/>
+      <c r="B16" s="37"/>
       <c r="C16" t="str">
         <f t="shared" si="1"/>
         <v>001110</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2904,7 +2904,7 @@
         <f t="shared" si="0"/>
         <v>0F</v>
       </c>
-      <c r="B17" s="36"/>
+      <c r="B17" s="37"/>
       <c r="C17" t="str">
         <f t="shared" si="1"/>
         <v>001111</v>
@@ -2913,10 +2913,10 @@
         <v>173</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2924,19 +2924,19 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B18" s="36"/>
+      <c r="B18" s="37"/>
       <c r="C18" t="str">
         <f t="shared" si="1"/>
         <v>010000</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2944,7 +2944,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="37"/>
       <c r="C19" t="str">
         <f t="shared" si="1"/>
         <v>010001</v>
@@ -2953,16 +2953,16 @@
         <v>224</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>228</v>
       </c>
       <c r="G19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H19" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2970,7 +2970,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B20" s="36"/>
+      <c r="B20" s="37"/>
       <c r="C20" t="str">
         <f t="shared" si="1"/>
         <v>010010</v>
@@ -2979,13 +2979,13 @@
         <v>225</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>229</v>
       </c>
       <c r="G20" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="H20" t="s">
         <v>232</v>
@@ -2996,7 +2996,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B21" s="36"/>
+      <c r="B21" s="37"/>
       <c r="C21" t="str">
         <f t="shared" si="1"/>
         <v>010011</v>
@@ -3005,10 +3005,10 @@
         <v>183</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -3016,7 +3016,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B22" s="36"/>
+      <c r="B22" s="37"/>
       <c r="C22" t="str">
         <f t="shared" si="1"/>
         <v>010100</v>
@@ -3031,7 +3031,7 @@
         <v>211</v>
       </c>
       <c r="H22" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -3039,7 +3039,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B23" s="36"/>
+      <c r="B23" s="37"/>
       <c r="C23" t="str">
         <f t="shared" si="1"/>
         <v>010101</v>
@@ -3054,7 +3054,7 @@
         <v>212</v>
       </c>
       <c r="H23" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3062,7 +3062,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B24" s="36"/>
+      <c r="B24" s="37"/>
       <c r="C24" t="str">
         <f t="shared" si="1"/>
         <v>010110</v>
@@ -3077,10 +3077,10 @@
         <v>213</v>
       </c>
       <c r="G24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H24" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -3088,7 +3088,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B25" s="36"/>
+      <c r="B25" s="37"/>
       <c r="C25" t="str">
         <f t="shared" si="1"/>
         <v>010111</v>
@@ -3103,10 +3103,10 @@
         <v>214</v>
       </c>
       <c r="G25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H25" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -3114,22 +3114,22 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B26" s="36"/>
+      <c r="B26" s="37"/>
       <c r="C26" t="str">
         <f t="shared" si="1"/>
         <v>011000</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>177</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H26" t="s">
         <v>195</v>
@@ -3140,25 +3140,25 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B27" s="36"/>
+      <c r="B27" s="37"/>
       <c r="C27" t="str">
         <f t="shared" si="1"/>
         <v>011001</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H27" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -3166,22 +3166,22 @@
         <f t="shared" si="0"/>
         <v>1A</v>
       </c>
-      <c r="B28" s="36"/>
+      <c r="B28" s="37"/>
       <c r="C28" t="str">
         <f t="shared" si="1"/>
         <v>011010</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>177</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H28" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3189,7 +3189,7 @@
         <f t="shared" si="0"/>
         <v>1B</v>
       </c>
-      <c r="B29" s="36"/>
+      <c r="B29" s="37"/>
       <c r="C29" t="str">
         <f t="shared" si="1"/>
         <v>011011</v>
@@ -3201,10 +3201,10 @@
         <v>177</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H29" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3212,7 +3212,7 @@
         <f t="shared" si="0"/>
         <v>1C</v>
       </c>
-      <c r="B30" s="36"/>
+      <c r="B30" s="37"/>
       <c r="C30" t="str">
         <f t="shared" si="1"/>
         <v>011100</v>
@@ -3224,10 +3224,10 @@
         <v>177</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H30" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -3235,22 +3235,22 @@
         <f t="shared" si="0"/>
         <v>1D</v>
       </c>
-      <c r="B31" s="36"/>
+      <c r="B31" s="37"/>
       <c r="C31" t="str">
         <f t="shared" si="1"/>
         <v>011101</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>177</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H31" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3258,22 +3258,22 @@
         <f t="shared" si="0"/>
         <v>1E</v>
       </c>
-      <c r="B32" s="36"/>
+      <c r="B32" s="37"/>
       <c r="C32" t="str">
         <f t="shared" si="1"/>
         <v>011110</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>177</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H32" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3281,22 +3281,22 @@
         <f t="shared" si="0"/>
         <v>1F</v>
       </c>
-      <c r="B33" s="36"/>
+      <c r="B33" s="37"/>
       <c r="C33" t="str">
         <f t="shared" si="1"/>
         <v>011111</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>177</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H33" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3304,13 +3304,13 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B34" s="36"/>
+      <c r="B34" s="37"/>
       <c r="C34" t="str">
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>215</v>
@@ -3319,10 +3319,10 @@
         <v>217</v>
       </c>
       <c r="G34" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="H34" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3330,25 +3330,25 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B35" s="36"/>
+      <c r="B35" s="37"/>
       <c r="C35" t="str">
         <f t="shared" si="1"/>
         <v>100001</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>194</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G35" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="H35" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3356,25 +3356,25 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B36" s="36"/>
+      <c r="B36" s="37"/>
       <c r="C36" t="str">
         <f t="shared" si="1"/>
         <v>100010</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>215</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G36" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="H36" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -3382,25 +3382,25 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B37" s="36"/>
+      <c r="B37" s="37"/>
       <c r="C37" t="str">
         <f t="shared" si="1"/>
         <v>100011</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>194</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G37" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="H37" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -3408,19 +3408,19 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B38" s="36"/>
+      <c r="B38" s="37"/>
       <c r="C38" t="str">
         <f t="shared" si="1"/>
         <v>100100</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>215</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="H38" t="s">
         <v>216</v>
@@ -3431,22 +3431,22 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B39" s="36"/>
+      <c r="B39" s="37"/>
       <c r="C39" t="str">
         <f t="shared" si="1"/>
         <v>100101</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>215</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="H39" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3454,22 +3454,22 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B40" s="36"/>
+      <c r="B40" s="37"/>
       <c r="C40" t="str">
         <f t="shared" si="1"/>
         <v>100110</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>215</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="H40" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -3477,22 +3477,22 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B41" s="36"/>
+      <c r="B41" s="37"/>
       <c r="C41" t="str">
         <f t="shared" si="1"/>
         <v>100111</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>215</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="H41" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3500,22 +3500,22 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B42" s="36"/>
+      <c r="B42" s="37"/>
       <c r="C42" t="str">
         <f t="shared" si="1"/>
         <v>101000</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>215</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="H42" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3523,22 +3523,22 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B43" s="36"/>
+      <c r="B43" s="37"/>
       <c r="C43" t="str">
         <f t="shared" si="1"/>
         <v>101001</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>215</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="H43" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3546,7 +3546,7 @@
         <f t="shared" si="0"/>
         <v>2A</v>
       </c>
-      <c r="B44" s="36"/>
+      <c r="B44" s="37"/>
       <c r="C44" t="str">
         <f t="shared" si="1"/>
         <v>101010</v>
@@ -3558,10 +3558,10 @@
         <v>189</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="H44" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3569,7 +3569,7 @@
         <f t="shared" si="0"/>
         <v>2B</v>
       </c>
-      <c r="B45" s="36"/>
+      <c r="B45" s="37"/>
       <c r="C45" t="str">
         <f t="shared" si="1"/>
         <v>101011</v>
@@ -3581,13 +3581,13 @@
         <v>191</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="G45" t="s">
         <v>192</v>
       </c>
       <c r="H45" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -3595,25 +3595,25 @@
         <f t="shared" si="0"/>
         <v>2C</v>
       </c>
-      <c r="B46" s="36"/>
+      <c r="B46" s="37"/>
       <c r="C46" t="str">
         <f t="shared" si="1"/>
         <v>101100</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E46" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="F46" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="F46" s="4" t="s">
-        <v>342</v>
-      </c>
       <c r="G46" s="4" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3621,28 +3621,28 @@
         <f t="shared" si="0"/>
         <v>2D</v>
       </c>
-      <c r="B47" s="36"/>
+      <c r="B47" s="37"/>
       <c r="C47" t="str">
         <f t="shared" si="1"/>
         <v>101101</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>196</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="G47" t="s">
         <v>197</v>
       </c>
       <c r="H47" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I47" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -3650,28 +3650,28 @@
         <f t="shared" si="0"/>
         <v>2E</v>
       </c>
-      <c r="B48" s="36"/>
+      <c r="B48" s="37"/>
       <c r="C48" t="str">
         <f t="shared" si="1"/>
         <v>101110</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>196</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G48" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="H48" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="I48" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3679,7 +3679,7 @@
         <f t="shared" si="0"/>
         <v>2F</v>
       </c>
-      <c r="B49" s="36"/>
+      <c r="B49" s="37"/>
       <c r="C49" t="str">
         <f t="shared" si="1"/>
         <v>101111</v>
@@ -3690,7 +3690,7 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B50" s="36"/>
+      <c r="B50" s="37"/>
       <c r="C50" t="str">
         <f t="shared" si="1"/>
         <v>110000</v>
@@ -3701,7 +3701,7 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B51" s="36"/>
+      <c r="B51" s="37"/>
       <c r="C51" t="str">
         <f t="shared" si="1"/>
         <v>110001</v>
@@ -3712,7 +3712,7 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B52" s="36"/>
+      <c r="B52" s="37"/>
       <c r="C52" t="str">
         <f t="shared" si="1"/>
         <v>110010</v>
@@ -3723,7 +3723,7 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B53" s="37"/>
+      <c r="B53" s="38"/>
       <c r="C53" t="str">
         <f t="shared" si="1"/>
         <v>110011</v>
@@ -3734,7 +3734,7 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B54" s="33" t="s">
+      <c r="B54" s="34" t="s">
         <v>145</v>
       </c>
       <c r="C54" t="str">
@@ -3745,13 +3745,13 @@
         <v>181</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>147</v>
       </c>
       <c r="H54" s="26" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3759,7 +3759,7 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B55" s="34"/>
+      <c r="B55" s="35"/>
       <c r="C55" t="str">
         <f t="shared" si="1"/>
         <v>110101</v>
@@ -3768,13 +3768,13 @@
         <v>184</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H55" s="26" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3782,7 +3782,7 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B56" s="34"/>
+      <c r="B56" s="35"/>
       <c r="C56" t="str">
         <f t="shared" si="1"/>
         <v>110110</v>
@@ -3791,7 +3791,7 @@
         <v>142</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>143</v>
@@ -3802,7 +3802,7 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B57" s="35"/>
+      <c r="B57" s="36"/>
       <c r="C57" t="str">
         <f t="shared" si="1"/>
         <v>110111</v>
@@ -3811,7 +3811,7 @@
         <v>185</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>144</v>
@@ -3822,7 +3822,7 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B58" s="32" t="s">
+      <c r="B58" s="33" t="s">
         <v>109</v>
       </c>
       <c r="C58" t="str">
@@ -3830,19 +3830,19 @@
         <v>111000</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3850,25 +3850,25 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B59" s="32"/>
+      <c r="B59" s="33"/>
       <c r="C59" t="str">
         <f t="shared" si="1"/>
         <v>111001</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3876,25 +3876,25 @@
         <f t="shared" si="0"/>
         <v>3A</v>
       </c>
-      <c r="B60" s="32"/>
+      <c r="B60" s="33"/>
       <c r="C60" t="str">
         <f t="shared" si="1"/>
         <v>111010</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3902,25 +3902,25 @@
         <f t="shared" si="0"/>
         <v>3B</v>
       </c>
-      <c r="B61" s="32"/>
+      <c r="B61" s="33"/>
       <c r="C61" t="str">
         <f t="shared" si="1"/>
         <v>111011</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3928,28 +3928,28 @@
         <f t="shared" si="0"/>
         <v>3C</v>
       </c>
-      <c r="B62" s="32"/>
+      <c r="B62" s="33"/>
       <c r="C62" t="str">
         <f t="shared" si="1"/>
         <v>111100</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>189</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3957,28 +3957,28 @@
         <f t="shared" si="0"/>
         <v>3D</v>
       </c>
-      <c r="B63" s="32"/>
+      <c r="B63" s="33"/>
       <c r="C63" t="str">
         <f t="shared" si="1"/>
         <v>111101</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>189</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3986,28 +3986,28 @@
         <f t="shared" si="0"/>
         <v>3E</v>
       </c>
-      <c r="B64" s="32"/>
+      <c r="B64" s="33"/>
       <c r="C64" t="str">
         <f t="shared" si="1"/>
         <v>111110</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>189</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -4015,28 +4015,28 @@
         <f t="shared" si="0"/>
         <v>3F</v>
       </c>
-      <c r="B65" s="32"/>
+      <c r="B65" s="33"/>
       <c r="C65" t="str">
         <f t="shared" si="1"/>
         <v>111111</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>189</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -4096,10 +4096,10 @@
         <v>115</v>
       </c>
       <c r="D1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E1" t="s">
         <v>239</v>
-      </c>
-      <c r="E1" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4133,7 +4133,7 @@
         <v>92</v>
       </c>
       <c r="E3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -4150,7 +4150,7 @@
         <v>211</v>
       </c>
       <c r="E4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -4201,7 +4201,7 @@
         <v>92</v>
       </c>
       <c r="E7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -4218,7 +4218,7 @@
         <v>211</v>
       </c>
       <c r="E8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -4235,12 +4235,12 @@
         <v>211</v>
       </c>
       <c r="E9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D10" s="24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -4285,18 +4285,18 @@
       <c r="E1" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
@@ -4702,11 +4702,11 @@
         <f t="shared" si="3"/>
         <v>00010000</v>
       </c>
-      <c r="J16" s="38" t="s">
+      <c r="J16" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
@@ -4728,8 +4728,8 @@
         <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="F17" s="42" t="s">
-        <v>390</v>
+      <c r="F17" s="41" t="s">
+        <v>386</v>
       </c>
       <c r="J17" t="s">
         <v>149</v>
@@ -4742,7 +4742,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F18" s="42"/>
+      <c r="F18" s="41"/>
       <c r="J18">
         <v>0</v>
       </c>
@@ -4754,7 +4754,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F19" s="42"/>
+      <c r="F19" s="41"/>
       <c r="J19">
         <v>0</v>
       </c>
@@ -4766,7 +4766,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F20" s="42"/>
+      <c r="F20" s="41"/>
       <c r="J20">
         <v>1</v>
       </c>
@@ -4781,12 +4781,12 @@
       <c r="A21" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="43" t="s">
-        <v>384</v>
-      </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
+      <c r="B21" s="40" t="s">
+        <v>380</v>
+      </c>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
       <c r="J21">
         <v>1</v>
       </c>
@@ -4798,52 +4798,52 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B27" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B28" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B29" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B30" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -4864,7 +4864,7 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4942,14 +4942,14 @@
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="M2" s="39" t="s">
+      <c r="M2" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
@@ -4961,10 +4961,10 @@
         <v>0001</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -5156,10 +5156,10 @@
         <v>0111</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
         <v>59</v>
@@ -5177,14 +5177,14 @@
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="M9" s="39" t="s">
+      <c r="M9" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="42"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
@@ -5318,11 +5318,11 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5431,7 +5431,7 @@
   <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5463,15 +5463,15 @@
       <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -5553,15 +5553,15 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J8" s="39" t="s">
+      <c r="J8" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="42"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
@@ -5573,10 +5573,10 @@
       <c r="L9" t="s">
         <v>50</v>
       </c>
-      <c r="M9" s="39" t="s">
+      <c r="M9" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="N9" s="39"/>
+      <c r="N9" s="42"/>
       <c r="P9" t="s">
         <v>57</v>
       </c>
@@ -5593,10 +5593,10 @@
       <c r="L10">
         <v>2</v>
       </c>
-      <c r="M10" s="39">
+      <c r="M10" s="42">
         <v>8</v>
       </c>
-      <c r="N10" s="39"/>
+      <c r="N10" s="42"/>
       <c r="P10">
         <f>SUM(K10:N10)</f>
         <v>16</v>
@@ -5611,15 +5611,15 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J15" s="40" t="s">
+      <c r="J15" s="43" t="s">
         <v>198</v>
       </c>
-      <c r="K15" s="40"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="40"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="40"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J16" s="5" t="s">

</xml_diff>

<commit_message>
Poprawki debugera: * Czytanie ramu i romu * Dodano zapis ramu * Dodano zapis rejestrów
Poprawki testów game padów
</commit_message>
<xml_diff>
--- a/KPC8/Docs/Specs.xlsx
+++ b/KPC8/Docs/Specs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Random\KPC8\KPC8\KPC8\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\KPC8\KPC8\KPC8\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85539B9-10FB-429F-8B63-BE61268E70DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D61B6CC-A5F6-4B2D-89D3-8B2CB25FF2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{17029D09-6E3C-4208-87C0-FA3EA582112B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="8" xr2:uid="{17029D09-6E3C-4208-87C0-FA3EA582112B}"/>
   </bookViews>
   <sheets>
     <sheet name="Control signals" sheetId="4" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="Registers" sheetId="2" r:id="rId5"/>
     <sheet name="Flags" sheetId="5" r:id="rId6"/>
     <sheet name="Instruction formats" sheetId="3" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="451">
   <si>
     <t>OPCODE HEX</t>
   </si>
@@ -1231,13 +1233,175 @@
   </si>
   <si>
     <t>Store byte RAM offset</t>
+  </si>
+  <si>
+    <t>FCEUX NES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MasterGear </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IodineGBA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GateBoy </t>
+  </si>
+  <si>
+    <t>LAYSIM-leon3</t>
+  </si>
+  <si>
+    <t>PIC CPU emulator</t>
+  </si>
+  <si>
+    <t>MC88110 CPU emulator</t>
+  </si>
+  <si>
+    <t>Emulator name</t>
+  </si>
+  <si>
+    <t>Goal/Focus</t>
+  </si>
+  <si>
+    <t>Gaming</t>
+  </si>
+  <si>
+    <t>Gaming, ROM hacking</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Hobbyist research</t>
+  </si>
+  <si>
+    <t>Flight software dev.</t>
+  </si>
+  <si>
+    <t>Program analysis</t>
+  </si>
+  <si>
+    <t>Emulation abstraction level</t>
+  </si>
+  <si>
+    <t>Cycle-true instruction set emulation</t>
+  </si>
+  <si>
+    <t>Emulation level description</t>
+  </si>
+  <si>
+    <t>Middle-high</t>
+  </si>
+  <si>
+    <t>Gate-level</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Functional units and behavior emulation</t>
+  </si>
+  <si>
+    <t>Middle</t>
+  </si>
+  <si>
+    <t>Emulation based on state transition system</t>
+  </si>
+  <si>
+    <t>Instruction set emulation</t>
+  </si>
+  <si>
+    <t>Not documented; source code not available</t>
+  </si>
+  <si>
+    <t>Not documented</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>CPU design</t>
+  </si>
+  <si>
+    <t>CPU emulation</t>
+  </si>
+  <si>
+    <t>CPU lighweight emulation</t>
+  </si>
+  <si>
+    <t>KPC8 assembly language</t>
+  </si>
+  <si>
+    <t>Debugger</t>
+  </si>
+  <si>
+    <t>Language support tools</t>
+  </si>
+  <si>
+    <t>Graphics card</t>
+  </si>
+  <si>
+    <t>Exemplary games and programs</t>
+  </si>
+  <si>
+    <t>Mobile application</t>
+  </si>
+  <si>
+    <t>Games store/marketplace</t>
+  </si>
+  <si>
+    <t>Online documentation</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>100% ready</t>
+  </si>
+  <si>
+    <t>Planned</t>
+  </si>
+  <si>
+    <t>80% ready</t>
+  </si>
+  <si>
+    <t>More pseudoinstructions to implement</t>
+  </si>
+  <si>
+    <t>90% ready</t>
+  </si>
+  <si>
+    <t>Stack frame contexts to be implemented</t>
+  </si>
+  <si>
+    <t>70% ready</t>
+  </si>
+  <si>
+    <t>Missing documentation and advanced features</t>
+  </si>
+  <si>
+    <t>Camera scrolling to be implemented</t>
+  </si>
+  <si>
+    <t>60% ready</t>
+  </si>
+  <si>
+    <t>More well-documented examples for beginners</t>
+  </si>
+  <si>
+    <t>For mobile device use</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1288,6 +1452,23 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -1516,9 +1697,8 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1534,7 +1714,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -1561,9 +1740,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1619,6 +1795,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
@@ -1631,7 +1809,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -1648,6 +1826,44 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1659,6 +1875,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AA295F00-2964-4479-94D0-D002B8A50608}" name="Table1" displayName="Table1" ref="A1:E8" totalsRowShown="0">
+  <autoFilter ref="A1:E8" xr:uid="{AA295F00-2964-4479-94D0-D002B8A50608}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E8">
+    <sortCondition ref="E1:E8"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{8E94E977-D52F-49B5-84CE-ED510A569365}" name="Emulator name" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{5C608F37-7ECC-48EF-9BDD-CEED38C56A8F}" name="Goal/Focus" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{EE15D57D-1E3F-4F8A-88FB-41EB5D908F5C}" name="Emulation level description"/>
+    <tableColumn id="4" xr3:uid="{1E65C965-1C42-420B-9E62-6FC03DFA89E7}" name="Emulation abstraction level"/>
+    <tableColumn id="5" xr3:uid="{0C0946D3-4B6E-4FCF-88CC-EA7165EBBA37}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1950,7 +2183,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1974,22 +2207,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1998,7 +2231,7 @@
         <f>ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="26" t="s">
         <v>94</v>
       </c>
       <c r="D2" t="s">
@@ -2013,7 +2246,7 @@
         <f t="shared" ref="A3:A32" si="0">ROW()-1</f>
         <v>2</v>
       </c>
-      <c r="C3" s="30"/>
+      <c r="C3" s="27"/>
       <c r="D3" t="s">
         <v>65</v>
       </c>
@@ -2026,7 +2259,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="27"/>
       <c r="D4" t="s">
         <v>65</v>
       </c>
@@ -2039,7 +2272,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C5" s="30"/>
+      <c r="C5" s="27"/>
       <c r="D5" t="s">
         <v>65</v>
       </c>
@@ -2052,7 +2285,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="27"/>
       <c r="D6" t="s">
         <v>66</v>
       </c>
@@ -2065,7 +2298,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C7" s="30"/>
+      <c r="C7" s="27"/>
       <c r="D7" t="s">
         <v>66</v>
       </c>
@@ -2078,7 +2311,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C8" s="30"/>
+      <c r="C8" s="27"/>
       <c r="D8" t="s">
         <v>66</v>
       </c>
@@ -2094,7 +2327,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C9" s="30"/>
+      <c r="C9" s="27"/>
       <c r="D9" t="s">
         <v>79</v>
       </c>
@@ -2107,7 +2340,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C10" s="30"/>
+      <c r="C10" s="27"/>
       <c r="D10" t="s">
         <v>66</v>
       </c>
@@ -2120,7 +2353,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C11" s="30"/>
+      <c r="C11" s="27"/>
       <c r="D11" t="s">
         <v>46</v>
       </c>
@@ -2133,7 +2366,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C12" s="30"/>
+      <c r="C12" s="27"/>
       <c r="D12" t="s">
         <v>46</v>
       </c>
@@ -2146,7 +2379,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C13" s="30"/>
+      <c r="C13" s="27"/>
       <c r="D13" t="s">
         <v>47</v>
       </c>
@@ -2159,7 +2392,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="28" t="s">
         <v>95</v>
       </c>
       <c r="D14" t="s">
@@ -2174,7 +2407,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C15" s="31"/>
+      <c r="C15" s="28"/>
       <c r="D15" t="s">
         <v>75</v>
       </c>
@@ -2187,7 +2420,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C16" s="31"/>
+      <c r="C16" s="28"/>
       <c r="D16" t="s">
         <v>75</v>
       </c>
@@ -2203,7 +2436,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C17" s="31"/>
+      <c r="C17" s="28"/>
       <c r="D17" t="s">
         <v>80</v>
       </c>
@@ -2216,7 +2449,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C18" s="31"/>
+      <c r="C18" s="28"/>
       <c r="D18" t="s">
         <v>81</v>
       </c>
@@ -2232,7 +2465,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C19" s="31"/>
+      <c r="C19" s="28"/>
       <c r="D19" t="s">
         <v>81</v>
       </c>
@@ -2245,7 +2478,7 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C20" s="31"/>
+      <c r="C20" s="28"/>
       <c r="D20" t="s">
         <v>96</v>
       </c>
@@ -2258,7 +2491,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C21" s="31"/>
+      <c r="C21" s="28"/>
       <c r="D21" t="s">
         <v>97</v>
       </c>
@@ -2271,7 +2504,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C22" s="31"/>
+      <c r="C22" s="28"/>
       <c r="D22" t="s">
         <v>98</v>
       </c>
@@ -2284,7 +2517,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C23" s="33" t="s">
+      <c r="C23" s="30" t="s">
         <v>82</v>
       </c>
       <c r="D23" t="s">
@@ -2299,7 +2532,7 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C24" s="33"/>
+      <c r="C24" s="30"/>
       <c r="D24" t="s">
         <v>82</v>
       </c>
@@ -2312,7 +2545,7 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="29" t="s">
         <v>83</v>
       </c>
       <c r="D25" t="s">
@@ -2327,7 +2560,7 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C26" s="32"/>
+      <c r="C26" s="29"/>
       <c r="D26" t="s">
         <v>73</v>
       </c>
@@ -2343,7 +2576,7 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C27" s="32"/>
+      <c r="C27" s="29"/>
       <c r="D27" t="s">
         <v>76</v>
       </c>
@@ -2356,7 +2589,7 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="C28" s="32"/>
+      <c r="C28" s="29"/>
       <c r="D28" t="s">
         <v>74</v>
       </c>
@@ -2369,7 +2602,7 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C29" s="32"/>
+      <c r="C29" s="29"/>
       <c r="D29" t="s">
         <v>74</v>
       </c>
@@ -2385,7 +2618,7 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="C30" s="32"/>
+      <c r="C30" s="29"/>
       <c r="D30" t="s">
         <v>78</v>
       </c>
@@ -2398,7 +2631,7 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="C31" s="32"/>
+      <c r="C31" s="29"/>
       <c r="D31" t="s">
         <v>83</v>
       </c>
@@ -2411,7 +2644,7 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="C32" s="32"/>
+      <c r="C32" s="29"/>
       <c r="D32" t="s">
         <v>83</v>
       </c>
@@ -2421,36 +2654,35 @@
     </row>
     <row r="33" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8" t="s">
+      <c r="C34" s="7"/>
+      <c r="D34" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E34" s="8">
         <f>COUNT(A:A)</f>
         <v>31</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11" t="s">
+      <c r="B35" s="9"/>
+      <c r="D35" t="s">
         <v>88</v>
       </c>
-      <c r="E35" s="12">
+      <c r="E35" s="10">
         <f>COUNTIF(F:F,"const 1")</f>
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="13"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14" t="s">
+      <c r="B36" s="11"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="13">
         <f>E34-E35</f>
         <v>26</v>
       </c>
@@ -2490,10 +2722,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F904DBB9-1FEB-4077-A5E6-86A97D866F70}">
-  <dimension ref="A1:W70"/>
+  <dimension ref="A1:W65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2501,8 +2733,8 @@
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
     <col min="2" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="38.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="38.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="53" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="51.5703125" customWidth="1"/>
     <col min="9" max="9" width="31.5703125" customWidth="1"/>
@@ -2526,19 +2758,19 @@
       <c r="D1" t="s">
         <v>175</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>40</v>
       </c>
       <c r="H1" t="s">
         <v>200</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>54</v>
       </c>
       <c r="W1" t="s">
@@ -2546,24 +2778,24 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="str">
+      <c r="A2" t="str">
         <f>DEC2HEX(_xlfn.NUMBERVALUE( ROW()-2),2)</f>
         <v>00</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="35" t="s">
         <v>108</v>
       </c>
       <c r="C2" t="str">
         <f>HEX2BIN(A2,6)</f>
         <v>000000</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>61</v>
       </c>
       <c r="W2" t="s">
@@ -2571,25 +2803,25 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="str">
+      <c r="A3" t="str">
         <f t="shared" ref="A3:A65" si="0">DEC2HEX(_xlfn.NUMBERVALUE( ROW()-2),2)</f>
         <v>01</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="35"/>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C65" si="1">HEX2BIN(A3,6)</f>
         <v>000001</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>168</v>
       </c>
       <c r="H3" t="s">
@@ -2600,55 +2832,55 @@
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="str">
+      <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>02</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="35"/>
       <c r="C4" t="str">
         <f t="shared" si="1"/>
         <v>000010</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="H4" t="s">
         <v>302</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="3"/>
       <c r="W4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="str">
+      <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>03</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="35"/>
       <c r="C5" t="str">
         <f t="shared" si="1"/>
         <v>000011</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>169</v>
       </c>
       <c r="H5" t="s">
@@ -2656,25 +2888,25 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="str">
+      <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>04</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="35"/>
       <c r="C6" t="str">
         <f t="shared" si="1"/>
         <v>000100</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>305</v>
       </c>
       <c r="H6" t="s">
@@ -2682,25 +2914,25 @@
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="str">
+      <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>05</v>
       </c>
-      <c r="B7" s="38"/>
+      <c r="B7" s="35"/>
       <c r="C7" t="str">
         <f t="shared" si="1"/>
         <v>000101</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>62</v>
       </c>
       <c r="H7" t="s">
@@ -2708,25 +2940,25 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="str">
+      <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>06</v>
       </c>
-      <c r="B8" s="38"/>
+      <c r="B8" s="35"/>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
         <v>000110</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>222</v>
       </c>
       <c r="H8" t="s">
@@ -2734,25 +2966,25 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="str">
+      <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>07</v>
       </c>
-      <c r="B9" s="38"/>
+      <c r="B9" s="35"/>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
         <v>000111</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>167</v>
       </c>
       <c r="H9" t="s">
@@ -2760,25 +2992,25 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="str">
+      <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>08</v>
       </c>
-      <c r="B10" s="38"/>
+      <c r="B10" s="35"/>
       <c r="C10" t="str">
         <f t="shared" si="1"/>
         <v>001000</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="20" t="s">
         <v>309</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>308</v>
       </c>
       <c r="H10" t="s">
@@ -2786,22 +3018,22 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="str">
+      <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>09</v>
       </c>
-      <c r="B11" s="38"/>
+      <c r="B11" s="35"/>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
         <v>001001</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>230</v>
       </c>
       <c r="G11" t="s">
@@ -2812,22 +3044,22 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="str">
+      <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>0A</v>
       </c>
-      <c r="B12" s="38"/>
+      <c r="B12" s="35"/>
       <c r="C12" t="str">
         <f t="shared" si="1"/>
         <v>001010</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>231</v>
       </c>
       <c r="G12" t="s">
@@ -2838,142 +3070,142 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="str">
+      <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>0B</v>
       </c>
-      <c r="B13" s="38"/>
+      <c r="B13" s="35"/>
       <c r="C13" t="str">
         <f t="shared" si="1"/>
         <v>001011</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="str">
+      <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>0C</v>
       </c>
-      <c r="B14" s="38"/>
+      <c r="B14" s="35"/>
       <c r="C14" t="str">
         <f t="shared" si="1"/>
         <v>001100</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="str">
+      <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>0D</v>
       </c>
-      <c r="B15" s="38"/>
+      <c r="B15" s="35"/>
       <c r="C15" t="str">
         <f t="shared" si="1"/>
         <v>001101</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="str">
+      <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>0E</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="35"/>
       <c r="C16" t="str">
         <f t="shared" si="1"/>
         <v>001110</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="20" t="s">
         <v>310</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="str">
+      <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>0F</v>
       </c>
-      <c r="B17" s="38"/>
+      <c r="B17" s="35"/>
       <c r="C17" t="str">
         <f t="shared" si="1"/>
         <v>001111</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="str">
+      <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B18" s="38"/>
+      <c r="B18" s="35"/>
       <c r="C18" t="str">
         <f t="shared" si="1"/>
         <v>010000</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="20" t="s">
         <v>311</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="str">
+      <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B19" s="38"/>
+      <c r="B19" s="35"/>
       <c r="C19" t="str">
         <f t="shared" si="1"/>
         <v>010001</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="20" t="s">
         <v>224</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>228</v>
       </c>
       <c r="G19" t="s">
@@ -2984,22 +3216,22 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="str">
+      <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="35"/>
       <c r="C20" t="str">
         <f t="shared" si="1"/>
         <v>010010</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="3" t="s">
         <v>229</v>
       </c>
       <c r="G20" t="s">
@@ -3010,42 +3242,42 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="str">
+      <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B21" s="38"/>
+      <c r="B21" s="35"/>
       <c r="C21" t="str">
         <f t="shared" si="1"/>
         <v>010011</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="str">
+      <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B22" s="38"/>
+      <c r="B22" s="35"/>
       <c r="C22" t="str">
         <f t="shared" si="1"/>
         <v>010100</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>211</v>
       </c>
       <c r="H22" t="s">
@@ -3053,22 +3285,22 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="str">
+      <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B23" s="38"/>
+      <c r="B23" s="35"/>
       <c r="C23" t="str">
         <f t="shared" si="1"/>
         <v>010101</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="3" t="s">
         <v>212</v>
       </c>
       <c r="H23" t="s">
@@ -3076,22 +3308,22 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="str">
+      <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B24" s="38"/>
+      <c r="B24" s="35"/>
       <c r="C24" t="str">
         <f t="shared" si="1"/>
         <v>010110</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="3" t="s">
         <v>213</v>
       </c>
       <c r="G24" t="s">
@@ -3102,22 +3334,22 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="str">
+      <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B25" s="38"/>
+      <c r="B25" s="35"/>
       <c r="C25" t="str">
         <f t="shared" si="1"/>
         <v>010111</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="3" t="s">
         <v>214</v>
       </c>
       <c r="G25" t="s">
@@ -3128,22 +3360,22 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="str">
+      <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B26" s="38"/>
+      <c r="B26" s="35"/>
       <c r="C26" t="str">
         <f t="shared" si="1"/>
         <v>011000</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>252</v>
       </c>
       <c r="G26" t="s">
@@ -3154,22 +3386,22 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="str">
+      <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B27" s="38"/>
+      <c r="B27" s="35"/>
       <c r="C27" t="str">
         <f t="shared" si="1"/>
         <v>011001</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="20" t="s">
         <v>255</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="3" t="s">
         <v>253</v>
       </c>
       <c r="G27" t="s">
@@ -3180,22 +3412,22 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="str">
+      <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>1A</v>
       </c>
-      <c r="B28" s="38"/>
+      <c r="B28" s="35"/>
       <c r="C28" t="str">
         <f t="shared" si="1"/>
         <v>011010</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="3" t="s">
         <v>247</v>
       </c>
       <c r="H28" t="s">
@@ -3203,22 +3435,22 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="str">
+      <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>1B</v>
       </c>
-      <c r="B29" s="38"/>
+      <c r="B29" s="35"/>
       <c r="C29" t="str">
         <f t="shared" si="1"/>
         <v>011011</v>
       </c>
-      <c r="D29" s="22" t="s">
+      <c r="D29" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="3" t="s">
         <v>246</v>
       </c>
       <c r="H29" t="s">
@@ -3226,22 +3458,22 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="str">
+      <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>1C</v>
       </c>
-      <c r="B30" s="38"/>
+      <c r="B30" s="35"/>
       <c r="C30" t="str">
         <f t="shared" si="1"/>
         <v>011100</v>
       </c>
-      <c r="D30" s="22" t="s">
+      <c r="D30" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="3" t="s">
         <v>244</v>
       </c>
       <c r="H30" t="s">
@@ -3249,22 +3481,22 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="str">
+      <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>1D</v>
       </c>
-      <c r="B31" s="38"/>
+      <c r="B31" s="35"/>
       <c r="C31" t="str">
         <f t="shared" si="1"/>
         <v>011101</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="3" t="s">
         <v>245</v>
       </c>
       <c r="H31" t="s">
@@ -3272,22 +3504,22 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="str">
+      <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>1E</v>
       </c>
-      <c r="B32" s="38"/>
+      <c r="B32" s="35"/>
       <c r="C32" t="str">
         <f t="shared" si="1"/>
         <v>011110</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="3" t="s">
         <v>243</v>
       </c>
       <c r="H32" t="s">
@@ -3295,22 +3527,22 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="str">
+      <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>1F</v>
       </c>
-      <c r="B33" s="38"/>
+      <c r="B33" s="35"/>
       <c r="C33" t="str">
         <f t="shared" si="1"/>
         <v>011111</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D33" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F33" s="3" t="s">
         <v>242</v>
       </c>
       <c r="H33" t="s">
@@ -3318,22 +3550,22 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="str">
+      <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B34" s="38"/>
+      <c r="B34" s="35"/>
       <c r="C34" t="str">
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="20" t="s">
         <v>267</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="F34" s="3" t="s">
         <v>217</v>
       </c>
       <c r="G34" t="s">
@@ -3344,22 +3576,22 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="str">
+      <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B35" s="38"/>
+      <c r="B35" s="35"/>
       <c r="C35" t="str">
         <f t="shared" si="1"/>
         <v>100001</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="3" t="s">
         <v>259</v>
       </c>
       <c r="G35" t="s">
@@ -3370,22 +3602,22 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="str">
+      <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B36" s="38"/>
+      <c r="B36" s="35"/>
       <c r="C36" t="str">
         <f t="shared" si="1"/>
         <v>100010</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="20" t="s">
         <v>268</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="3" t="s">
         <v>276</v>
       </c>
       <c r="G36" t="s">
@@ -3396,22 +3628,22 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="str">
+      <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B37" s="38"/>
+      <c r="B37" s="35"/>
       <c r="C37" t="str">
         <f t="shared" si="1"/>
         <v>100011</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D37" s="20" t="s">
         <v>258</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="3" t="s">
         <v>260</v>
       </c>
       <c r="G37" t="s">
@@ -3422,22 +3654,22 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="str">
+      <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B38" s="38"/>
+      <c r="B38" s="35"/>
       <c r="C38" t="str">
         <f t="shared" si="1"/>
         <v>100100</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="20" t="s">
         <v>269</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="3" t="s">
         <v>290</v>
       </c>
       <c r="H38" t="s">
@@ -3445,22 +3677,22 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="str">
+      <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B39" s="38"/>
+      <c r="B39" s="35"/>
       <c r="C39" t="str">
         <f t="shared" si="1"/>
         <v>100101</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F39" s="3" t="s">
         <v>292</v>
       </c>
       <c r="H39" t="s">
@@ -3468,22 +3700,22 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="str">
+      <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B40" s="38"/>
+      <c r="B40" s="35"/>
       <c r="C40" t="str">
         <f t="shared" si="1"/>
         <v>100110</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D40" s="20" t="s">
         <v>266</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="3" t="s">
         <v>291</v>
       </c>
       <c r="H40" t="s">
@@ -3491,22 +3723,22 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="str">
+      <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B41" s="38"/>
+      <c r="B41" s="35"/>
       <c r="C41" t="str">
         <f t="shared" si="1"/>
         <v>100111</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="D41" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="3" t="s">
         <v>293</v>
       </c>
       <c r="H41" t="s">
@@ -3514,22 +3746,22 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="str">
+      <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B42" s="38"/>
+      <c r="B42" s="35"/>
       <c r="C42" t="str">
         <f t="shared" si="1"/>
         <v>101000</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D42" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F42" s="3" t="s">
         <v>294</v>
       </c>
       <c r="H42" t="s">
@@ -3537,22 +3769,22 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="str">
+      <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B43" s="38"/>
+      <c r="B43" s="35"/>
       <c r="C43" t="str">
         <f t="shared" si="1"/>
         <v>101001</v>
       </c>
-      <c r="D43" s="22" t="s">
+      <c r="D43" s="20" t="s">
         <v>270</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F43" s="3" t="s">
         <v>295</v>
       </c>
       <c r="H43" t="s">
@@ -3560,22 +3792,22 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="str">
+      <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>2A</v>
       </c>
-      <c r="B44" s="38"/>
+      <c r="B44" s="35"/>
       <c r="C44" t="str">
         <f t="shared" si="1"/>
         <v>101010</v>
       </c>
-      <c r="D44" s="22" t="s">
+      <c r="D44" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="3" t="s">
         <v>299</v>
       </c>
       <c r="H44" t="s">
@@ -3583,22 +3815,22 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="str">
+      <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>2B</v>
       </c>
-      <c r="B45" s="38"/>
+      <c r="B45" s="35"/>
       <c r="C45" t="str">
         <f t="shared" si="1"/>
         <v>101011</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D45" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F45" s="3" t="s">
         <v>300</v>
       </c>
       <c r="G45" t="s">
@@ -3609,48 +3841,48 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="str">
+      <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>2C</v>
       </c>
-      <c r="B46" s="38"/>
+      <c r="B46" s="35"/>
       <c r="C46" t="str">
         <f t="shared" si="1"/>
         <v>101100</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D46" s="20" t="s">
         <v>334</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F46" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="G46" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="H46" s="4" t="s">
+      <c r="H46" s="3" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="str">
+      <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>2D</v>
       </c>
-      <c r="B47" s="38"/>
+      <c r="B47" s="35"/>
       <c r="C47" t="str">
         <f t="shared" si="1"/>
         <v>101101</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="20" t="s">
         <v>329</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="F47" s="3" t="s">
         <v>336</v>
       </c>
       <c r="G47" t="s">
@@ -3664,22 +3896,22 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="str">
+      <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>2E</v>
       </c>
-      <c r="B48" s="38"/>
+      <c r="B48" s="35"/>
       <c r="C48" t="str">
         <f t="shared" si="1"/>
         <v>101110</v>
       </c>
-      <c r="D48" s="22" t="s">
+      <c r="D48" s="20" t="s">
         <v>330</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F48" s="3" t="s">
         <v>337</v>
       </c>
       <c r="G48" t="s">
@@ -3693,395 +3925,375 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="str">
+      <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>2F</v>
       </c>
-      <c r="B49" s="38"/>
+      <c r="B49" s="35"/>
       <c r="C49" t="str">
         <f t="shared" si="1"/>
         <v>101111</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="str">
+      <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B50" s="38"/>
+      <c r="B50" s="35"/>
       <c r="C50" t="str">
         <f t="shared" si="1"/>
         <v>110000</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="str">
+      <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B51" s="38"/>
+      <c r="B51" s="35"/>
       <c r="C51" t="str">
         <f t="shared" si="1"/>
         <v>110001</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="str">
+      <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B52" s="38"/>
+      <c r="B52" s="35"/>
       <c r="C52" t="str">
         <f t="shared" si="1"/>
         <v>110010</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="str">
+      <c r="A53" t="str">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B53" s="39"/>
+      <c r="B53" s="36"/>
       <c r="C53" t="str">
         <f t="shared" si="1"/>
         <v>110011</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="str">
+      <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B54" s="35" t="s">
+      <c r="B54" s="32" t="s">
         <v>145</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="1"/>
         <v>110100</v>
       </c>
-      <c r="D54" s="22" t="s">
+      <c r="D54" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="F54" s="28" t="s">
+      <c r="F54" s="25" t="s">
         <v>393</v>
       </c>
-      <c r="G54" s="4" t="s">
+      <c r="G54" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="H54" s="26" t="s">
+      <c r="H54" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="I54" s="26" t="s">
+      <c r="I54" s="3" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="str">
+      <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B55" s="36"/>
+      <c r="B55" s="33"/>
       <c r="C55" t="str">
         <f t="shared" si="1"/>
         <v>110101</v>
       </c>
-      <c r="D55" s="22" t="s">
+      <c r="D55" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E55" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="G55" s="4" t="s">
+      <c r="G55" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="H55" s="26" t="s">
+      <c r="H55" s="3" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="str">
+      <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B56" s="36"/>
+      <c r="B56" s="33"/>
       <c r="C56" t="str">
         <f t="shared" si="1"/>
         <v>110110</v>
       </c>
-      <c r="D56" s="22" t="s">
+      <c r="D56" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="E56" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="G56" s="4" t="s">
+      <c r="G56" s="3" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="str">
+      <c r="A57" t="str">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B57" s="37"/>
+      <c r="B57" s="34"/>
       <c r="C57" t="str">
         <f t="shared" si="1"/>
         <v>110111</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="D57" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E57" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="G57" s="4" t="s">
+      <c r="G57" s="3" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="str">
+      <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B58" s="34" t="s">
+      <c r="B58" s="31" t="s">
         <v>109</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="1"/>
         <v>111000</v>
       </c>
-      <c r="D58" s="22" t="s">
+      <c r="D58" s="20" t="s">
         <v>338</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E58" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="F58" s="4" t="s">
+      <c r="F58" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="G58" s="4" t="s">
+      <c r="G58" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="H58" s="4" t="s">
+      <c r="H58" s="3" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="str">
+      <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B59" s="34"/>
+      <c r="B59" s="31"/>
       <c r="C59" t="str">
         <f t="shared" si="1"/>
         <v>111001</v>
       </c>
-      <c r="D59" s="22" t="s">
+      <c r="D59" s="20" t="s">
         <v>352</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E59" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="F59" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="G59" s="4" t="s">
+      <c r="G59" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="H59" s="4" t="s">
+      <c r="H59" s="3" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="str">
+      <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>3A</v>
       </c>
-      <c r="B60" s="34"/>
+      <c r="B60" s="31"/>
       <c r="C60" t="str">
         <f t="shared" si="1"/>
         <v>111010</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="D60" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="E60" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="F60" s="4" t="s">
+      <c r="F60" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="G60" s="4" t="s">
+      <c r="G60" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="H60" s="4" t="s">
+      <c r="H60" s="3" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="str">
+      <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>3B</v>
       </c>
-      <c r="B61" s="34"/>
+      <c r="B61" s="31"/>
       <c r="C61" t="str">
         <f t="shared" si="1"/>
         <v>111011</v>
       </c>
-      <c r="D61" s="22" t="s">
+      <c r="D61" s="20" t="s">
         <v>358</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E61" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="F61" s="4" t="s">
+      <c r="F61" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="G61" s="4" t="s">
+      <c r="G61" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="H61" s="4" t="s">
+      <c r="H61" s="3" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="str">
+      <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>3C</v>
       </c>
-      <c r="B62" s="34"/>
+      <c r="B62" s="31"/>
       <c r="C62" t="str">
         <f t="shared" si="1"/>
         <v>111100</v>
       </c>
-      <c r="D62" s="22" t="s">
+      <c r="D62" s="20" t="s">
         <v>346</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="E62" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="F62" s="4" t="s">
+      <c r="F62" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="G62" s="4" t="s">
+      <c r="G62" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="H62" s="4" t="s">
+      <c r="H62" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="I62" s="4" t="s">
+      <c r="I62" s="3" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="str">
+      <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>3D</v>
       </c>
-      <c r="B63" s="34"/>
+      <c r="B63" s="31"/>
       <c r="C63" t="str">
         <f t="shared" si="1"/>
         <v>111101</v>
       </c>
-      <c r="D63" s="22" t="s">
+      <c r="D63" s="20" t="s">
         <v>347</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E63" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="F63" s="4" t="s">
+      <c r="F63" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="G63" s="4" t="s">
+      <c r="G63" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="H63" s="4" t="s">
+      <c r="H63" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="I63" s="4" t="s">
+      <c r="I63" s="3" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="str">
+      <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>3E</v>
       </c>
-      <c r="B64" s="34"/>
+      <c r="B64" s="31"/>
       <c r="C64" t="str">
         <f t="shared" si="1"/>
         <v>111110</v>
       </c>
-      <c r="D64" s="22" t="s">
+      <c r="D64" s="20" t="s">
         <v>342</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E64" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="F64" s="4" t="s">
+      <c r="F64" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="G64" s="4" t="s">
+      <c r="G64" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="H64" s="4" t="s">
+      <c r="H64" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="I64" s="4" t="s">
+      <c r="I64" s="3" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="str">
+      <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>3F</v>
       </c>
-      <c r="B65" s="34"/>
+      <c r="B65" s="31"/>
       <c r="C65" t="str">
         <f t="shared" si="1"/>
         <v>111111</v>
       </c>
-      <c r="D65" s="22" t="s">
+      <c r="D65" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E65" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="F65" s="4" t="s">
+      <c r="F65" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G65" s="4" t="s">
+      <c r="G65" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="H65" s="4" t="s">
+      <c r="H65" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="I65" s="4" t="s">
+      <c r="I65" s="3" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4136,10 +4348,10 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>92</v>
       </c>
     </row>
@@ -4153,7 +4365,7 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="22" t="s">
         <v>92</v>
       </c>
       <c r="E3" t="s">
@@ -4170,7 +4382,7 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="18" t="s">
         <v>211</v>
       </c>
       <c r="E4" t="s">
@@ -4187,7 +4399,7 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="22" t="s">
         <v>92</v>
       </c>
       <c r="E5" t="s">
@@ -4204,7 +4416,7 @@
       <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="22" t="s">
         <v>92</v>
       </c>
       <c r="E6" t="s">
@@ -4221,7 +4433,7 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="22" t="s">
         <v>92</v>
       </c>
       <c r="E7" t="s">
@@ -4238,7 +4450,7 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="18" t="s">
         <v>211</v>
       </c>
       <c r="E8" t="s">
@@ -4255,7 +4467,7 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="18" t="s">
         <v>211</v>
       </c>
       <c r="E9" t="s">
@@ -4263,7 +4475,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="22" t="s">
         <v>250</v>
       </c>
     </row>
@@ -4294,33 +4506,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
@@ -4483,19 +4695,19 @@
         <f t="shared" si="3"/>
         <v>10110000</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="L6" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="N6" s="15" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4519,10 +4731,10 @@
         <f t="shared" si="3"/>
         <v>10100000</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="17" t="s">
         <v>138</v>
       </c>
     </row>
@@ -4549,13 +4761,13 @@
       <c r="J8" t="s">
         <v>137</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="L8" s="18" t="s">
+      <c r="L8" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="M8" s="18" t="s">
+      <c r="M8" s="16" t="s">
         <v>160</v>
       </c>
     </row>
@@ -4726,33 +4938,33 @@
         <f t="shared" si="3"/>
         <v>00010000</v>
       </c>
-      <c r="J16" s="40" t="s">
+      <c r="J16" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="str">
+      <c r="A17" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0F</v>
       </c>
-      <c r="B17" s="5" t="str">
+      <c r="B17" s="4" t="str">
         <f t="shared" si="1"/>
         <v>1111</v>
       </c>
-      <c r="C17" s="5" t="str">
+      <c r="C17" s="4" t="str">
         <f t="shared" si="2"/>
         <v>FF00</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>11010000</v>
       </c>
-      <c r="E17" s="5" t="str">
+      <c r="E17" s="4" t="str">
         <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="39" t="s">
         <v>382</v>
       </c>
       <c r="J17" t="s">
@@ -4766,7 +4978,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F18" s="42"/>
+      <c r="F18" s="39"/>
       <c r="J18">
         <v>0</v>
       </c>
@@ -4778,7 +4990,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F19" s="42"/>
+      <c r="F19" s="39"/>
       <c r="J19">
         <v>0</v>
       </c>
@@ -4790,7 +5002,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F20" s="42"/>
+      <c r="F20" s="39"/>
       <c r="J20">
         <v>1</v>
       </c>
@@ -4805,12 +5017,12 @@
       <c r="A21" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="38" t="s">
         <v>377</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
       <c r="J21">
         <v>1</v>
       </c>
@@ -4822,16 +5034,16 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -4842,29 +5054,29 @@
       <c r="A27" t="s">
         <v>375</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="21" t="s">
         <v>376</v>
       </c>
-      <c r="C27" s="43" t="s">
+      <c r="C27" s="40" t="s">
         <v>388</v>
       </c>
-      <c r="D27" s="41" t="s">
+      <c r="D27" s="38" t="s">
         <v>389</v>
       </c>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>373</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="21" t="s">
         <v>374</v>
       </c>
-      <c r="C28" s="43"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -4912,47 +5124,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="I1" s="6" t="s">
+      <c r="F1" s="5"/>
+      <c r="I1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>123</v>
       </c>
     </row>
@@ -4980,14 +5192,14 @@
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="M2" s="44" t="s">
+      <c r="M2" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="44"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
@@ -5215,14 +5427,14 @@
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="M9" s="44" t="s">
+      <c r="M9" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="N9" s="44"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="44"/>
-      <c r="Q9" s="44"/>
-      <c r="R9" s="44"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="41"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
@@ -5356,11 +5568,11 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5501,15 +5713,15 @@
       <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="44" t="s">
+      <c r="J1" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -5591,15 +5803,15 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J8" s="44" t="s">
+      <c r="J8" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="44"/>
-      <c r="N8" s="44"/>
-      <c r="O8" s="44"/>
-      <c r="P8" s="44"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
@@ -5611,15 +5823,15 @@
       <c r="L9" t="s">
         <v>50</v>
       </c>
-      <c r="M9" s="44" t="s">
+      <c r="M9" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="N9" s="44"/>
+      <c r="N9" s="41"/>
       <c r="P9" t="s">
         <v>57</v>
       </c>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
@@ -5631,10 +5843,10 @@
       <c r="L10">
         <v>2</v>
       </c>
-      <c r="M10" s="44">
+      <c r="M10" s="41">
         <v>8</v>
       </c>
-      <c r="N10" s="44"/>
+      <c r="N10" s="41"/>
       <c r="P10">
         <f>SUM(K10:N10)</f>
         <v>16</v>
@@ -5649,76 +5861,76 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J15" s="45" t="s">
+      <c r="J15" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="K15" s="45"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="45"/>
-      <c r="O15" s="45"/>
-      <c r="P15" s="45"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="42"/>
+      <c r="N15" s="42"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="42"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J16" s="5" t="s">
+      <c r="J16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="L16" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="M16" s="25" t="s">
+      <c r="M16" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="N16" s="25" t="s">
+      <c r="N16" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5" t="s">
+      <c r="O16" s="4"/>
+      <c r="P16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
     </row>
     <row r="17" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J17" s="5" t="s">
+      <c r="J17" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="K17" s="5">
+      <c r="K17" s="4">
         <v>6</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="4">
         <v>2</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="23">
         <v>4</v>
       </c>
-      <c r="N17" s="25">
+      <c r="N17" s="23">
         <v>4</v>
       </c>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5">
+      <c r="O17" s="4"/>
+      <c r="P17" s="4">
         <f>SUM(K17:N17)</f>
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5" t="s">
+      <c r="K18" s="4"/>
+      <c r="L18" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
     </row>
     <row r="27" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="K27" s="16"/>
+      <c r="K27" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5730,4 +5942,302 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8465B43-39E7-46F3-9A90-026902CC812B}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D1" t="s">
+        <v>412</v>
+      </c>
+      <c r="E1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>400</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>409</v>
+      </c>
+      <c r="C2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>397</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>407</v>
+      </c>
+      <c r="C3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D3" t="s">
+        <v>420</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>403</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>408</v>
+      </c>
+      <c r="C4" t="s">
+        <v>419</v>
+      </c>
+      <c r="D4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
+        <v>401</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>410</v>
+      </c>
+      <c r="C5" t="s">
+        <v>413</v>
+      </c>
+      <c r="D5" t="s">
+        <v>415</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
+        <v>402</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>411</v>
+      </c>
+      <c r="C6" t="s">
+        <v>421</v>
+      </c>
+      <c r="D6" t="s">
+        <v>415</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
+        <v>399</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>406</v>
+      </c>
+      <c r="C7" t="s">
+        <v>422</v>
+      </c>
+      <c r="D7" t="s">
+        <v>418</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>398</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>406</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>423</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>424</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD19A8A2-DD86-4598-8907-F6EC414A23A5}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B3" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>430</v>
+      </c>
+      <c r="B4" t="s">
+        <v>443</v>
+      </c>
+      <c r="C4" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>432</v>
+      </c>
+      <c r="B5" t="s">
+        <v>443</v>
+      </c>
+      <c r="C5" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>429</v>
+      </c>
+      <c r="B6" t="s">
+        <v>441</v>
+      </c>
+      <c r="C6" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>431</v>
+      </c>
+      <c r="B7" t="s">
+        <v>445</v>
+      </c>
+      <c r="C7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>433</v>
+      </c>
+      <c r="B8" t="s">
+        <v>448</v>
+      </c>
+      <c r="C8" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>428</v>
+      </c>
+      <c r="B9" t="s">
+        <v>440</v>
+      </c>
+      <c r="C9" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>434</v>
+      </c>
+      <c r="B10" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>435</v>
+      </c>
+      <c r="B11" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>436</v>
+      </c>
+      <c r="B12" t="s">
+        <v>440</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>